<commit_message>
Changed input file to add something
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Sablefish_ApportionmentStrategies\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18220" windowHeight="22080" tabRatio="694"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="22080" tabRatio="767"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -37,7 +42,7 @@
     <author>Curry Cunningham</author>
   </authors>
   <commentList>
-    <comment ref="C8" authorId="0">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +63,8 @@
           </rPr>
           <t xml:space="preserve">
 This was not listed in Kari's spreadsheet in Catchability Tab. Only USFish_postIFQ
-NEED TO DOUBLE CHECK!!!</t>
+NEED TO DOUBLE CHECK!!!
+There is not trawl fishery q in my spatial model.</t>
         </r>
       </text>
     </comment>
@@ -67,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="76">
   <si>
     <t>Par</t>
   </si>
@@ -277,13 +283,31 @@
   </si>
   <si>
     <t>n.year</t>
+  </si>
+  <si>
+    <t>n.length</t>
+  </si>
+  <si>
+    <t>Number of length bins</t>
+  </si>
+  <si>
+    <t>first.len</t>
+  </si>
+  <si>
+    <t>Smallest length bin label</t>
+  </si>
+  <si>
+    <t>len.incr</t>
+  </si>
+  <si>
+    <t>Length bin increment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -356,6 +380,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -377,8 +402,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,6 +442,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -522,7 +561,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -547,19 +586,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="40"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="40" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="3" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="3" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="40" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -634,6 +687,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -959,15 +1020,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -978,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -989,7 +1050,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1000,7 +1061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1072,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1022,15 +1083,48 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1045,15 +1139,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="C8" sqref="C8:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -1067,7 +1161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1075,10 +1169,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>2.1506150985899999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
@@ -1086,10 +1180,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>2.1506150985899999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -1097,40 +1191,106 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>2.1506150985899999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="21" t="s">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B8" s="19">
         <v>1</v>
       </c>
-      <c r="C5" s="21">
-        <v>1.6217900278699999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="21" t="s">
+      <c r="C8" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B9" s="19">
         <v>2</v>
       </c>
-      <c r="C6" s="21">
-        <v>1.6217900278699999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="21" t="s">
+      <c r="C9" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B10" s="19">
         <v>3</v>
       </c>
-      <c r="C7" s="21">
-        <v>1.6217900278699999</v>
+      <c r="C10" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="19">
+        <v>4</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="19">
+        <v>5</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="19">
+        <v>6</v>
+      </c>
+      <c r="C13" s="18">
+        <v>1.62</v>
       </c>
     </row>
   </sheetData>
@@ -1146,18 +1306,18 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -1177,8 +1337,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B2">
@@ -1188,14 +1348,14 @@
         <v>50</v>
       </c>
       <c r="D2" s="12">
-        <v>0.81613783000499995</v>
+        <v>0.83268153466700001</v>
       </c>
       <c r="E2" s="12">
-        <v>2.1707804981900001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="18" t="s">
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B3">
@@ -1211,8 +1371,8 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B4">
@@ -1224,8 +1384,8 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B5">
@@ -1235,14 +1395,14 @@
         <v>50</v>
       </c>
       <c r="D5" s="12">
-        <v>0.81613783000499995</v>
+        <v>0.83268153466700001</v>
       </c>
       <c r="E5" s="12">
-        <v>2.1707804981900001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="18" t="s">
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B6">
@@ -1258,8 +1418,8 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B7">
@@ -1271,8 +1431,8 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B8">
@@ -1282,14 +1442,14 @@
         <v>50</v>
       </c>
       <c r="D8" s="12">
-        <v>0.81613783000499995</v>
+        <v>0.83268153466700001</v>
       </c>
       <c r="E8" s="12">
-        <v>2.1707804981900001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="18" t="s">
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B9">
@@ -1305,8 +1465,8 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B10">
@@ -1318,76 +1478,76 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="11" t="s">
-        <v>67</v>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="16">
-        <v>0.84880840201200003</v>
-      </c>
-      <c r="E11" s="16">
-        <v>0.83233751308500004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="11" t="s">
-        <v>67</v>
+      <c r="D11" s="12">
+        <v>0.83268153466700001</v>
+      </c>
+      <c r="E11" s="12">
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E12" s="16">
-        <v>1.1394028495799999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="11" t="s">
-        <v>67</v>
+      <c r="E12" s="13">
+        <v>0.51393999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="11" t="s">
-        <v>67</v>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="12">
-        <v>1.12724360426</v>
+        <v>0.83268153466700001</v>
       </c>
       <c r="E14" s="12">
-        <v>1.1802557447599999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="11" t="s">
-        <v>67</v>
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -1396,15 +1556,15 @@
         <v>0.88417999999999997</v>
       </c>
       <c r="E15" s="13">
-        <v>1.1394028495799999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="11" t="s">
-        <v>67</v>
+        <v>0.51393999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
@@ -1412,56 +1572,56 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="11" t="s">
-        <v>67</v>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="14">
-        <v>1.4339075566299999</v>
-      </c>
-      <c r="E17" s="14">
-        <v>1.30680347891</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="11" t="s">
-        <v>67</v>
+      <c r="D17" s="12">
+        <v>0.83268153466700001</v>
+      </c>
+      <c r="E17" s="12">
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="13">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E18" s="14">
-        <v>1.1394028495799999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="11" t="s">
-        <v>67</v>
+      <c r="E18" s="13">
+        <v>0.51393999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1469,15 +1629,16 @@
       <c r="C20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="D20" s="20">
+        <v>0.85317342242799998</v>
+      </c>
+      <c r="E20" s="20">
+        <v>0.83233751308500004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1485,19 +1646,16 @@
       <c r="C21" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="12">
-        <v>1.41239440332</v>
-      </c>
-      <c r="E21" s="12">
-        <v>1.3242791632099999</v>
-      </c>
-      <c r="F21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="D21" s="20">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E21" s="20">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1505,19 +1663,12 @@
       <c r="C22" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="12">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="E22" s="13">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="F22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1525,15 +1676,16 @@
       <c r="C23" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="D23" s="22">
+        <v>0.85317342242799998</v>
+      </c>
+      <c r="E23" s="22">
+        <v>0.83233751308500004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1541,19 +1693,16 @@
       <c r="C24" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="12">
-        <v>1.41239440332</v>
-      </c>
-      <c r="E24" s="12">
-        <v>1.3242791632099999</v>
-      </c>
-      <c r="F24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="D24" s="23">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E24" s="23">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1561,19 +1710,12 @@
       <c r="C25" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="12">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="E25" s="13">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="F25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -1581,15 +1723,16 @@
       <c r="C26" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="D26" s="25">
+        <v>0.85317342242799998</v>
+      </c>
+      <c r="E26" s="25">
+        <v>0.83233751308500004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -1597,19 +1740,16 @@
       <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="12">
-        <v>1.41239440332</v>
-      </c>
-      <c r="E27" s="12">
-        <v>1.3242791632099999</v>
-      </c>
-      <c r="F27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="D27" s="26">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E27" s="25">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1617,159 +1757,770 @@
       <c r="C28" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="12">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="E28" s="13">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="F28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="14">
-        <v>2.1</v>
-      </c>
-      <c r="E29" s="14">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="D29" s="27">
+        <v>1.1324375825599999</v>
+      </c>
+      <c r="E29" s="27">
+        <v>1.1762722908800001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-      <c r="E30" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="D30" s="26">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E30" s="25">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="14">
-        <v>2.1</v>
-      </c>
-      <c r="E32" s="14">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="D32" s="25">
+        <v>1.4339075566299999</v>
+      </c>
+      <c r="E32" s="27">
+        <v>1.29701630606</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-      <c r="E33" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="D33" s="26">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E33" s="25">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="14">
-        <v>2.1</v>
-      </c>
-      <c r="E35" s="14">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="D35" s="25">
+        <v>1.4339075566299999</v>
+      </c>
+      <c r="E35" s="27">
+        <v>1.29701630606</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-      <c r="E36" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="D36" s="26">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E36" s="25">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E39" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E40" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E42" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E43" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E45" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E46" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E48" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E49" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E51" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E52" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E54" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D55" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E55" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D56" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E56" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E57" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>50</v>
+      </c>
+      <c r="D59" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E59" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E60" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>50</v>
+      </c>
+      <c r="D62" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E62" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>51</v>
+      </c>
+      <c r="D63" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E63" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>50</v>
+      </c>
+      <c r="D65" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E65" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>51</v>
+      </c>
+      <c r="D66" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E66" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>50</v>
+      </c>
+      <c r="D68" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E68" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>51</v>
+      </c>
+      <c r="D69" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E69" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B70">
+        <v>5</v>
+      </c>
+      <c r="C70" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71">
+        <v>6</v>
+      </c>
+      <c r="C71" t="s">
+        <v>50</v>
+      </c>
+      <c r="D71" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E71" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>51</v>
+      </c>
+      <c r="D72" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E72" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73">
+        <v>6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>52</v>
+      </c>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A37">
+  <conditionalFormatting sqref="B2:B37">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1781,7 +2532,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B19">
+  <conditionalFormatting sqref="B38:B55">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1793,7 +2544,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20:B28">
+  <conditionalFormatting sqref="B56:B73">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1805,7 +2556,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:B37">
+  <conditionalFormatting sqref="A2:A55 A65:A73">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:A64">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1832,15 +2595,15 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1">
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -1848,35 +2611,35 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1904,18 +2667,18 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -1929,143 +2692,272 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>1.66374977939</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="18" t="s">
+        <v>1.7069903579000001</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>1.1217419339000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="18" t="s">
+        <v>1.7069903579000001</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>1.2124099417400001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="12" t="s">
+        <v>1.7069903579000001</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1.1852290194399999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1.29233648959</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1.29233648959</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B8" s="9">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
-        <v>1.70430230078</v>
-      </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="12" t="s">
+      <c r="C8" s="7">
+        <v>1.7026485760600001</v>
+      </c>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B9" s="9">
         <v>2</v>
       </c>
-      <c r="C6" s="7">
-        <v>1.63169859462</v>
-      </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="12" t="s">
+      <c r="C9" s="7">
+        <v>1.7026485760600001</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B10" s="9">
         <v>3</v>
       </c>
-      <c r="C7" s="7">
-        <v>2.0490144139200002</v>
-      </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+      <c r="C10" s="7">
+        <v>1.7026485760600001</v>
+      </c>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="9">
+        <v>4</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1.6218141693999999</v>
+      </c>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="9">
+        <v>5</v>
+      </c>
+      <c r="C12" s="7">
+        <v>2.04462323042</v>
+      </c>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="9">
+        <v>6</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2.04462323042</v>
+      </c>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>57</v>
       </c>
-      <c r="B8">
+      <c r="B14">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
-        <v>1.70430230078</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>57</v>
       </c>
-      <c r="B9">
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C9" s="1">
-        <v>1.63169859462</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>57</v>
       </c>
-      <c r="B10">
+      <c r="B16">
         <v>3</v>
       </c>
-      <c r="C10" s="1">
-        <v>2.0490144139200002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="9" t="s">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B20" s="9">
         <v>1</v>
       </c>
-      <c r="C11" s="7">
-        <v>2.6315002330800001</v>
-      </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="9" t="s">
+      <c r="C20" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B21" s="9">
         <v>2</v>
       </c>
-      <c r="C12" s="7">
-        <v>2.6315002330800001</v>
-      </c>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="9" t="s">
+      <c r="C21" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B22" s="9">
         <v>3</v>
       </c>
-      <c r="C13" s="7">
-        <v>2.6315002330800001</v>
-      </c>
-      <c r="D13" s="9"/>
+      <c r="C22" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="9">
+        <v>4</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="9">
+        <v>5</v>
+      </c>
+      <c r="C24" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="9">
+        <v>6</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D25" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
@@ -2092,7 +2984,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
+  <conditionalFormatting sqref="A4:A7">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2104,7 +2996,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
+  <conditionalFormatting sqref="A8">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2116,7 +3008,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
+  <conditionalFormatting sqref="A9">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2128,7 +3020,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
+  <conditionalFormatting sqref="A10:A13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2159,7 +3051,7 @@
       <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2175,12 +3067,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2191,18 +3083,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -2213,12 +3105,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -2238,13 +3130,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2258,7 +3150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2272,7 +3164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2286,7 +3178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2300,7 +3192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -2314,7 +3206,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -2328,7 +3220,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2339,7 +3231,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -2350,7 +3242,7 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -2361,7 +3253,7 @@
         <v>0.35599999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -2390,9 +3282,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2406,7 +3298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -2423,7 +3315,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -2440,7 +3332,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2454,7 +3346,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2487,9 +3379,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2500,7 +3392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -2514,7 +3406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2525,7 +3417,7 @@
         <v>9.7500000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -2554,9 +3446,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2567,7 +3459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -2578,7 +3470,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2603,16 +3495,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2623,7 +3515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -2631,7 +3523,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2639,7 +3531,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2647,7 +3539,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -2669,16 +3561,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -2695,7 +3587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -2709,7 +3601,7 @@
         <v>1.16683899284</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
@@ -2723,7 +3615,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -2733,7 +3625,7 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
@@ -2747,7 +3639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -2761,7 +3653,7 @@
         <v>0.82430000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -2771,7 +3663,7 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
@@ -2785,7 +3677,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -2818,12 +3710,12 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -2831,7 +3723,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -2839,7 +3731,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Bringing up to date
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Sablefish_ApportionmentStrategies\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18220" windowHeight="22080" tabRatio="694"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="22080" tabRatio="767"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -37,7 +42,7 @@
     <author>Curry Cunningham</author>
   </authors>
   <commentList>
-    <comment ref="C8" authorId="0">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +63,8 @@
           </rPr>
           <t xml:space="preserve">
 This was not listed in Kari's spreadsheet in Catchability Tab. Only USFish_postIFQ
-NEED TO DOUBLE CHECK!!!</t>
+NEED TO DOUBLE CHECK!!!
+There is not trawl fishery q in my spatial model.</t>
         </r>
       </text>
     </comment>
@@ -67,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="78">
   <si>
     <t>Par</t>
   </si>
@@ -277,13 +283,37 @@
   </si>
   <si>
     <t>n.year</t>
+  </si>
+  <si>
+    <t>n.length</t>
+  </si>
+  <si>
+    <t>Number of length bins</t>
+  </si>
+  <si>
+    <t>first.len</t>
+  </si>
+  <si>
+    <t>Smallest length bin label</t>
+  </si>
+  <si>
+    <t>len.incr</t>
+  </si>
+  <si>
+    <t>Length bin increment</t>
+  </si>
+  <si>
+    <t>move.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 is single matrix (not age or time varying); </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -356,6 +386,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -377,8 +408,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,6 +448,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -522,7 +567,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -547,19 +592,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="40"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="40" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="3" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="3" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="40" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -634,6 +693,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -959,15 +1026,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -978,7 +1045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -989,7 +1056,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1000,7 +1067,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1078,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1022,15 +1089,59 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1045,15 +1156,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="C8" sqref="C8:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -1067,7 +1178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1075,10 +1186,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>2.1506150985899999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
@@ -1086,10 +1197,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>2.1506150985899999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -1097,40 +1208,106 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>2.1506150985899999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="21" t="s">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B8" s="19">
         <v>1</v>
       </c>
-      <c r="C5" s="21">
-        <v>1.6217900278699999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="21" t="s">
+      <c r="C8" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B9" s="19">
         <v>2</v>
       </c>
-      <c r="C6" s="21">
-        <v>1.6217900278699999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="21" t="s">
+      <c r="C9" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B10" s="19">
         <v>3</v>
       </c>
-      <c r="C7" s="21">
-        <v>1.6217900278699999</v>
+      <c r="C10" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="19">
+        <v>4</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="19">
+        <v>5</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="19">
+        <v>6</v>
+      </c>
+      <c r="C13" s="18">
+        <v>1.62</v>
       </c>
     </row>
   </sheetData>
@@ -1146,18 +1323,18 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -1177,8 +1354,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B2">
@@ -1188,14 +1365,14 @@
         <v>50</v>
       </c>
       <c r="D2" s="12">
-        <v>0.81613783000499995</v>
+        <v>0.83268153466700001</v>
       </c>
       <c r="E2" s="12">
-        <v>2.1707804981900001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="18" t="s">
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B3">
@@ -1211,8 +1388,8 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B4">
@@ -1224,8 +1401,8 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B5">
@@ -1235,14 +1412,14 @@
         <v>50</v>
       </c>
       <c r="D5" s="12">
-        <v>0.81613783000499995</v>
+        <v>0.83268153466700001</v>
       </c>
       <c r="E5" s="12">
-        <v>2.1707804981900001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="18" t="s">
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B6">
@@ -1258,8 +1435,8 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B7">
@@ -1271,8 +1448,8 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B8">
@@ -1282,14 +1459,14 @@
         <v>50</v>
       </c>
       <c r="D8" s="12">
-        <v>0.81613783000499995</v>
+        <v>0.83268153466700001</v>
       </c>
       <c r="E8" s="12">
-        <v>2.1707804981900001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="18" t="s">
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B9">
@@ -1305,8 +1482,8 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B10">
@@ -1318,76 +1495,76 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="11" t="s">
-        <v>67</v>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="16">
-        <v>0.84880840201200003</v>
-      </c>
-      <c r="E11" s="16">
-        <v>0.83233751308500004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="11" t="s">
-        <v>67</v>
+      <c r="D11" s="12">
+        <v>0.83268153466700001</v>
+      </c>
+      <c r="E11" s="12">
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E12" s="16">
-        <v>1.1394028495799999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="11" t="s">
-        <v>67</v>
+      <c r="E12" s="13">
+        <v>0.51393999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="11" t="s">
-        <v>67</v>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="12">
-        <v>1.12724360426</v>
+        <v>0.83268153466700001</v>
       </c>
       <c r="E14" s="12">
-        <v>1.1802557447599999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="11" t="s">
-        <v>67</v>
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -1396,15 +1573,15 @@
         <v>0.88417999999999997</v>
       </c>
       <c r="E15" s="13">
-        <v>1.1394028495799999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="11" t="s">
-        <v>67</v>
+        <v>0.51393999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
@@ -1412,56 +1589,56 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="11" t="s">
-        <v>67</v>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="14">
-        <v>1.4339075566299999</v>
-      </c>
-      <c r="E17" s="14">
-        <v>1.30680347891</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="11" t="s">
-        <v>67</v>
+      <c r="D17" s="12">
+        <v>0.83268153466700001</v>
+      </c>
+      <c r="E17" s="12">
+        <v>2.28448156415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="13">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E18" s="14">
-        <v>1.1394028495799999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="11" t="s">
-        <v>67</v>
+      <c r="E18" s="13">
+        <v>0.51393999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1469,15 +1646,16 @@
       <c r="C20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="D20" s="20">
+        <v>0.85317342242799998</v>
+      </c>
+      <c r="E20" s="20">
+        <v>0.83233751308500004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1485,19 +1663,16 @@
       <c r="C21" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="12">
-        <v>1.41239440332</v>
-      </c>
-      <c r="E21" s="12">
-        <v>1.3242791632099999</v>
-      </c>
-      <c r="F21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="D21" s="20">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E21" s="20">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1505,19 +1680,12 @@
       <c r="C22" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="12">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="E22" s="13">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="F22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1525,15 +1693,16 @@
       <c r="C23" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="D23" s="22">
+        <v>0.85317342242799998</v>
+      </c>
+      <c r="E23" s="22">
+        <v>0.83233751308500004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1541,19 +1710,16 @@
       <c r="C24" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="12">
-        <v>1.41239440332</v>
-      </c>
-      <c r="E24" s="12">
-        <v>1.3242791632099999</v>
-      </c>
-      <c r="F24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="D24" s="23">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E24" s="23">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1561,19 +1727,12 @@
       <c r="C25" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="12">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="E25" s="13">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="F25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -1581,15 +1740,16 @@
       <c r="C26" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="D26" s="25">
+        <v>0.85317342242799998</v>
+      </c>
+      <c r="E26" s="25">
+        <v>0.83233751308500004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -1597,19 +1757,16 @@
       <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="12">
-        <v>1.41239440332</v>
-      </c>
-      <c r="E27" s="12">
-        <v>1.3242791632099999</v>
-      </c>
-      <c r="F27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="D27" s="26">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E27" s="25">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1617,159 +1774,770 @@
       <c r="C28" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="12">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="E28" s="13">
-        <v>1.7420935928000001</v>
-      </c>
-      <c r="F28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="14">
-        <v>2.1</v>
-      </c>
-      <c r="E29" s="14">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="D29" s="27">
+        <v>1.1324375825599999</v>
+      </c>
+      <c r="E29" s="27">
+        <v>1.1762722908800001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-      <c r="E30" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="D30" s="26">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E30" s="25">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="14">
-        <v>2.1</v>
-      </c>
-      <c r="E32" s="14">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="D32" s="25">
+        <v>1.4339075566299999</v>
+      </c>
+      <c r="E32" s="27">
+        <v>1.29701630606</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-      <c r="E33" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="D33" s="26">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E33" s="25">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="14">
-        <v>2.1</v>
-      </c>
-      <c r="E35" s="14">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="D35" s="25">
+        <v>1.4339075566299999</v>
+      </c>
+      <c r="E35" s="27">
+        <v>1.29701630606</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-      <c r="E36" s="14">
-        <v>0.78649999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="D36" s="26">
+        <v>0.88417999999999997</v>
+      </c>
+      <c r="E36" s="25">
+        <v>1.1467086815500001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E39" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E40" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E42" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E43" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E45" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E46" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E48" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E49" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E51" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E52" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="12">
+        <v>1.4069980317499999</v>
+      </c>
+      <c r="E54" s="12">
+        <v>1.3394329648900001</v>
+      </c>
+      <c r="F54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D55" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="E55" s="12">
+        <v>1.74173878351</v>
+      </c>
+      <c r="F55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D56" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E56" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E57" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>50</v>
+      </c>
+      <c r="D59" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E59" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E60" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>50</v>
+      </c>
+      <c r="D62" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E62" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>51</v>
+      </c>
+      <c r="D63" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E63" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>50</v>
+      </c>
+      <c r="D65" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E65" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>51</v>
+      </c>
+      <c r="D66" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E66" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>50</v>
+      </c>
+      <c r="D68" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E68" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>51</v>
+      </c>
+      <c r="D69" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E69" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B70">
+        <v>5</v>
+      </c>
+      <c r="C70" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71">
+        <v>6</v>
+      </c>
+      <c r="C71" t="s">
+        <v>50</v>
+      </c>
+      <c r="D71" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="E71" s="14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>51</v>
+      </c>
+      <c r="D72" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="E72" s="14">
+        <v>0.78649999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73">
+        <v>6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>52</v>
+      </c>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A37">
+  <conditionalFormatting sqref="B2:B37">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1781,7 +2549,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B19">
+  <conditionalFormatting sqref="B38:B55">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1793,7 +2561,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20:B28">
+  <conditionalFormatting sqref="B56:B73">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1805,7 +2573,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:B37">
+  <conditionalFormatting sqref="A2:A55 A65:A73">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:A64">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1832,15 +2612,15 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1">
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -1848,35 +2628,35 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1904,18 +2684,18 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -1929,143 +2709,272 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>1.66374977939</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="18" t="s">
+        <v>1.7069903579000001</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>1.1217419339000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="18" t="s">
+        <v>1.7069903579000001</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>1.2124099417400001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="12" t="s">
+        <v>1.7069903579000001</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1.1852290194399999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1.29233648959</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1.29233648959</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B8" s="9">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
-        <v>1.70430230078</v>
-      </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="12" t="s">
+      <c r="C8" s="7">
+        <v>1.7026485760600001</v>
+      </c>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B9" s="9">
         <v>2</v>
       </c>
-      <c r="C6" s="7">
-        <v>1.63169859462</v>
-      </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="12" t="s">
+      <c r="C9" s="7">
+        <v>1.7026485760600001</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B10" s="9">
         <v>3</v>
       </c>
-      <c r="C7" s="7">
-        <v>2.0490144139200002</v>
-      </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+      <c r="C10" s="7">
+        <v>1.7026485760600001</v>
+      </c>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="9">
+        <v>4</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1.6218141693999999</v>
+      </c>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="9">
+        <v>5</v>
+      </c>
+      <c r="C12" s="7">
+        <v>2.04462323042</v>
+      </c>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="9">
+        <v>6</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2.04462323042</v>
+      </c>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>57</v>
       </c>
-      <c r="B8">
+      <c r="B14">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
-        <v>1.70430230078</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>57</v>
       </c>
-      <c r="B9">
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C9" s="1">
-        <v>1.63169859462</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>57</v>
       </c>
-      <c r="B10">
+      <c r="B16">
         <v>3</v>
       </c>
-      <c r="C10" s="1">
-        <v>2.0490144139200002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="9" t="s">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B20" s="9">
         <v>1</v>
       </c>
-      <c r="C11" s="7">
-        <v>2.6315002330800001</v>
-      </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="9" t="s">
+      <c r="C20" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B21" s="9">
         <v>2</v>
       </c>
-      <c r="C12" s="7">
-        <v>2.6315002330800001</v>
-      </c>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="9" t="s">
+      <c r="C21" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B22" s="9">
         <v>3</v>
       </c>
-      <c r="C13" s="7">
-        <v>2.6315002330800001</v>
-      </c>
-      <c r="D13" s="9"/>
+      <c r="C22" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="9">
+        <v>4</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="9">
+        <v>5</v>
+      </c>
+      <c r="C24" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="9">
+        <v>6</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2.6092073636799999</v>
+      </c>
+      <c r="D25" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
@@ -2092,7 +3001,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
+  <conditionalFormatting sqref="A4:A7">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2104,7 +3013,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
+  <conditionalFormatting sqref="A8">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2116,7 +3025,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
+  <conditionalFormatting sqref="A9">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2128,7 +3037,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
+  <conditionalFormatting sqref="A10:A13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2155,11 +3064,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2175,12 +3082,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2191,18 +3098,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -2213,12 +3120,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -2238,13 +3145,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2258,7 +3165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2272,7 +3179,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2286,7 +3193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2300,7 +3207,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -2314,7 +3221,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -2328,7 +3235,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2339,7 +3246,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -2350,7 +3257,7 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -2361,7 +3268,7 @@
         <v>0.35599999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -2390,9 +3297,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2406,7 +3313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -2423,7 +3330,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -2440,7 +3347,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2454,7 +3361,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2487,9 +3394,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2500,7 +3407,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -2514,7 +3421,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2525,7 +3432,7 @@
         <v>9.7500000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -2554,9 +3461,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2567,7 +3474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -2578,7 +3485,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2603,16 +3510,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2623,7 +3530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -2631,7 +3538,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2639,7 +3546,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2647,7 +3554,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -2669,16 +3576,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -2695,7 +3602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -2709,7 +3616,7 @@
         <v>1.16683899284</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
@@ -2723,7 +3630,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -2733,7 +3640,7 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
@@ -2747,7 +3654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -2761,7 +3668,7 @@
         <v>0.82430000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -2771,7 +3678,7 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
@@ -2785,7 +3692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -2818,12 +3725,12 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -2831,7 +3738,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -2839,7 +3746,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
added a (non-functioning) function to try to calculate F for the inital population set up.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,28 +9,30 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="22080" tabRatio="767" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="22080" tabRatio="767" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Sim" sheetId="4" r:id="rId2"/>
     <sheet name="Init_pop" sheetId="17" r:id="rId3"/>
     <sheet name="Init_pop_Rec" sheetId="18" r:id="rId4"/>
-    <sheet name="Init_pop_Catch" sheetId="19" r:id="rId5"/>
-    <sheet name="Growth" sheetId="2" r:id="rId6"/>
-    <sheet name="Maturity" sheetId="3" r:id="rId7"/>
-    <sheet name="Mortality" sheetId="5" r:id="rId8"/>
-    <sheet name="Recruitment" sheetId="6" r:id="rId9"/>
-    <sheet name="Catchability_SAFE" sheetId="7" r:id="rId10"/>
-    <sheet name="SurveySelectivity" sheetId="8" r:id="rId11"/>
-    <sheet name="SurveySelexType" sheetId="11" r:id="rId12"/>
-    <sheet name="qSurvey" sheetId="12" r:id="rId13"/>
-    <sheet name="FisherySelectivity" sheetId="9" r:id="rId14"/>
-    <sheet name="FisherySelexType" sheetId="14" r:id="rId15"/>
-    <sheet name="qFishery" sheetId="15" r:id="rId16"/>
-    <sheet name="Movement" sheetId="16" r:id="rId17"/>
+    <sheet name="Init_rec_prop" sheetId="20" r:id="rId5"/>
+    <sheet name="Init_pop_Catch" sheetId="19" r:id="rId6"/>
+    <sheet name="Init_fishAC" sheetId="21" r:id="rId7"/>
+    <sheet name="Growth" sheetId="2" r:id="rId8"/>
+    <sheet name="Maturity" sheetId="3" r:id="rId9"/>
+    <sheet name="Mortality" sheetId="5" r:id="rId10"/>
+    <sheet name="Recruitment" sheetId="6" r:id="rId11"/>
+    <sheet name="Catchability_SAFE" sheetId="7" r:id="rId12"/>
+    <sheet name="SurveySelectivity" sheetId="8" r:id="rId13"/>
+    <sheet name="SurveySelexType" sheetId="11" r:id="rId14"/>
+    <sheet name="qSurvey" sheetId="12" r:id="rId15"/>
+    <sheet name="FisherySelectivity" sheetId="9" r:id="rId16"/>
+    <sheet name="FisherySelexType" sheetId="14" r:id="rId17"/>
+    <sheet name="qFishery" sheetId="15" r:id="rId18"/>
+    <sheet name="Movement" sheetId="16" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -77,6 +79,77 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Kari.Fenske</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kari.Fenske:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+assumes 50:50 split for sex at recruitment age
+this is value for one sex, not sexes combined
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Kari.Fenske</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kari.Fenske:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+years 1979-2018
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
     <author>Curry Cunningham</author>
   </authors>
   <commentList>
@@ -111,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="103">
   <si>
     <t>Par</t>
   </si>
@@ -371,22 +444,64 @@
     <t>Year</t>
   </si>
   <si>
-    <t>FixedGearCatch</t>
-  </si>
-  <si>
-    <t>TrawlGearCatch</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>area1</t>
+  </si>
+  <si>
+    <t>area2</t>
+  </si>
+  <si>
+    <t>area3</t>
+  </si>
+  <si>
+    <t>area4</t>
+  </si>
+  <si>
+    <t>area5</t>
+  </si>
+  <si>
+    <t>area6</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>Fx_TrCatch_A1</t>
+  </si>
+  <si>
+    <t>Fx_TrCatch_A2</t>
+  </si>
+  <si>
+    <t>Fx_TrCatch_A3</t>
+  </si>
+  <si>
+    <t>Fx_TrCatch_A4</t>
+  </si>
+  <si>
+    <t>Fx_TrCatch_A5</t>
+  </si>
+  <si>
+    <t>Fx_TrCatch_A6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -654,7 +769,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -709,6 +824,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1246,6 +1362,126 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>0.1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>7.9500000000000001E-2</v>
+      </c>
+      <c r="C3">
+        <v>9.7500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>16.5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>1.2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -1310,7 +1546,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -1455,7 +1691,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1503,7 +1739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -1670,7 +1906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
@@ -2956,7 +3192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -3031,7 +3267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -3409,7 +3645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -3635,10 +3871,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P361"/>
+  <dimension ref="A1:E361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3654,10 +3890,10 @@
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3915,7 +4151,7 @@
         <v>0.21384566585956416</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1979</v>
       </c>
@@ -3931,19 +4167,8 @@
       <c r="E17" s="31">
         <v>0.62419815980629534</v>
       </c>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1979</v>
       </c>
@@ -3959,19 +4184,8 @@
       <c r="E18" s="31">
         <v>0.16760876513317191</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1979</v>
       </c>
@@ -3987,19 +4201,8 @@
       <c r="E19" s="31">
         <v>0.2774214043583535</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1979</v>
       </c>
@@ -4015,19 +4218,8 @@
       <c r="E20" s="31">
         <v>0.46986079903147693</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1979</v>
       </c>
@@ -4043,19 +4235,8 @@
       <c r="E21" s="31">
         <v>0.63808256658595641</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1979</v>
       </c>
@@ -4071,19 +4252,8 @@
       <c r="E22" s="31">
         <v>0.21462777239709444</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1979</v>
       </c>
@@ -4099,19 +4269,8 @@
       <c r="E23" s="31">
         <v>0.62648106537530268</v>
       </c>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1979</v>
       </c>
@@ -4127,19 +4286,8 @@
       <c r="E24" s="31">
         <v>0.1682217675544794</v>
       </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1979</v>
       </c>
@@ -4155,19 +4303,8 @@
       <c r="E25" s="31">
         <v>0.27843602905569004</v>
       </c>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1979</v>
       </c>
@@ -4183,19 +4320,8 @@
       <c r="E26" s="31">
         <v>0.34397542372881351</v>
       </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1979</v>
       </c>
@@ -4211,19 +4337,8 @@
       <c r="E27" s="31">
         <v>0.46712711864406781</v>
       </c>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1979</v>
       </c>
@@ -4239,19 +4354,8 @@
       <c r="E28" s="31">
         <v>0.15712457627118645</v>
       </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1979</v>
       </c>
@@ -4267,19 +4371,8 @@
       <c r="E29" s="31">
         <v>0.45863389830508472</v>
       </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1979</v>
       </c>
@@ -4295,19 +4388,8 @@
       <c r="E30" s="31">
         <v>0.12315169491525423</v>
       </c>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1979</v>
       </c>
@@ -4323,19 +4405,8 @@
       <c r="E31" s="31">
         <v>0.20383728813559321</v>
       </c>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="31"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1979</v>
       </c>
@@ -4351,19 +4422,8 @@
       <c r="E32" s="31">
         <v>0.3533600484261501</v>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1979</v>
       </c>
@@ -4379,19 +4439,8 @@
       <c r="E33" s="31">
         <v>0.47987167070217923</v>
       </c>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="31"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1979</v>
       </c>
@@ -4407,19 +4456,8 @@
       <c r="E34" s="31">
         <v>0.16141138014527848</v>
       </c>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="31"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1979</v>
       </c>
@@ -4435,19 +4473,8 @@
       <c r="E35" s="31">
         <v>0.47114673123486689</v>
       </c>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="31"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="31"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1979</v>
       </c>
@@ -4463,19 +4490,8 @@
       <c r="E36" s="31">
         <v>0.12651162227602905</v>
       </c>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="31"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1979</v>
       </c>
@@ -4491,19 +4507,8 @@
       <c r="E37" s="31">
         <v>0.20939854721549639</v>
       </c>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="31"/>
-      <c r="M37" s="31"/>
-      <c r="N37" s="31"/>
-      <c r="O37" s="31"/>
-      <c r="P37" s="31"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1979</v>
       </c>
@@ -4519,19 +4524,8 @@
       <c r="E38" s="31">
         <v>0.59458707021791768</v>
       </c>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="31"/>
-      <c r="L38" s="31"/>
-      <c r="M38" s="31"/>
-      <c r="N38" s="31"/>
-      <c r="O38" s="31"/>
-      <c r="P38" s="31"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1979</v>
       </c>
@@ -4547,19 +4541,8 @@
       <c r="E39" s="31">
         <v>0.80746392251815979</v>
       </c>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
-      <c r="L39" s="31"/>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
-      <c r="P39" s="31"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1979</v>
       </c>
@@ -4575,19 +4558,8 @@
       <c r="E40" s="31">
         <v>0.2716015012106538</v>
       </c>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31"/>
-      <c r="P40" s="31"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1979</v>
       </c>
@@ -4603,19 +4575,8 @@
       <c r="E41" s="31">
         <v>0.79278276029055694</v>
       </c>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
-      <c r="P41" s="31"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1979</v>
       </c>
@@ -4631,19 +4592,8 @@
       <c r="E42" s="31">
         <v>0.21287685230024211</v>
       </c>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
-      <c r="M42" s="31"/>
-      <c r="N42" s="31"/>
-      <c r="O42" s="31"/>
-      <c r="P42" s="31"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1979</v>
       </c>
@@ -4659,19 +4609,8 @@
       <c r="E43" s="31">
         <v>0.35234789346246975</v>
       </c>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
-      <c r="N43" s="31"/>
-      <c r="O43" s="31"/>
-      <c r="P43" s="31"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1979</v>
       </c>
@@ -4687,19 +4626,8 @@
       <c r="E44" s="31">
         <v>0.64763520581113798</v>
       </c>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
-      <c r="L44" s="31"/>
-      <c r="M44" s="31"/>
-      <c r="N44" s="31"/>
-      <c r="O44" s="31"/>
-      <c r="P44" s="31"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1979</v>
       </c>
@@ -4715,19 +4643,8 @@
       <c r="E45" s="31">
         <v>0.87950460048426149</v>
       </c>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="31"/>
-      <c r="L45" s="31"/>
-      <c r="M45" s="31"/>
-      <c r="N45" s="31"/>
-      <c r="O45" s="31"/>
-      <c r="P45" s="31"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1979</v>
       </c>
@@ -4743,19 +4660,8 @@
       <c r="E46" s="31">
         <v>0.29583336561743345</v>
       </c>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
-      <c r="N46" s="31"/>
-      <c r="O46" s="31"/>
-      <c r="P46" s="31"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1979</v>
       </c>
@@ -4772,7 +4678,7 @@
         <v>0.86351360774818409</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1979</v>
       </c>
@@ -10117,934 +10023,274 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AO1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1979</v>
-      </c>
-      <c r="B2">
         <v>43.192999999999998</v>
       </c>
-      <c r="C2">
-        <v>43.192999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1980</v>
-      </c>
-      <c r="B3">
         <v>12.71</v>
       </c>
-      <c r="C3">
-        <v>12.71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1981</v>
-      </c>
-      <c r="B4">
         <v>4.9525499999999996</v>
       </c>
-      <c r="C4">
-        <v>4.9525499999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1982</v>
-      </c>
-      <c r="B5">
         <v>21.151499999999999</v>
       </c>
-      <c r="C5">
-        <v>21.151499999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1983</v>
-      </c>
-      <c r="B6">
         <v>11.9864</v>
       </c>
-      <c r="C6">
-        <v>11.9864</v>
-      </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1984</v>
-      </c>
-      <c r="B7">
         <v>21.756900000000002</v>
       </c>
-      <c r="C7">
-        <v>21.756900000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1985</v>
-      </c>
-      <c r="B8">
         <v>1.1687399999999999</v>
       </c>
-      <c r="C8">
-        <v>1.1687399999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1986</v>
-      </c>
-      <c r="B9">
         <v>9.7652099999999997</v>
       </c>
-      <c r="C9">
-        <v>9.7652099999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1987</v>
-      </c>
-      <c r="B10">
         <v>9.4046099999999999</v>
       </c>
-      <c r="C10">
-        <v>9.4046099999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1988</v>
-      </c>
-      <c r="B11">
         <v>1.8113999999999999</v>
       </c>
-      <c r="C11">
-        <v>1.8113999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1989</v>
-      </c>
-      <c r="B12">
         <v>2.2608100000000002</v>
       </c>
-      <c r="C12">
-        <v>2.2608100000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1990</v>
-      </c>
-      <c r="B13">
         <v>3.4381300000000001</v>
       </c>
-      <c r="C13">
-        <v>3.4381300000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1991</v>
-      </c>
-      <c r="B14">
         <v>13.6341</v>
       </c>
-      <c r="C14">
-        <v>13.6341</v>
-      </c>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1992</v>
-      </c>
-      <c r="B15">
         <v>0.64316600000000002</v>
       </c>
-      <c r="C15">
-        <v>0.64316600000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1993</v>
-      </c>
-      <c r="B16">
         <v>11.894600000000001</v>
       </c>
-      <c r="C16">
-        <v>11.894600000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1994</v>
-      </c>
-      <c r="B17">
         <v>2.2991799999999998</v>
       </c>
-      <c r="C17">
-        <v>2.2991799999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1995</v>
-      </c>
-      <c r="B18">
         <v>2.6568200000000002</v>
       </c>
-      <c r="C18">
-        <v>2.6568200000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1996</v>
-      </c>
-      <c r="B19">
         <v>3.86592</v>
       </c>
-      <c r="C19">
-        <v>3.86592</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1997</v>
-      </c>
-      <c r="B20">
         <v>8.4420800000000007</v>
       </c>
-      <c r="C20">
-        <v>8.4420800000000007</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1998</v>
-      </c>
-      <c r="B21">
         <v>1.1508100000000001</v>
       </c>
-      <c r="C21">
-        <v>1.1508100000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1999</v>
-      </c>
-      <c r="B22">
         <v>14.961499999999999</v>
       </c>
-      <c r="C22">
-        <v>14.961499999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2000</v>
-      </c>
-      <c r="B23">
         <v>8.4678100000000001</v>
       </c>
-      <c r="C23">
-        <v>8.4678100000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2001</v>
-      </c>
-      <c r="B24">
         <v>5.0763299999999996</v>
       </c>
-      <c r="C24">
-        <v>5.0763299999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2002</v>
-      </c>
-      <c r="B25">
         <v>20.7346</v>
       </c>
-      <c r="C25">
-        <v>20.7346</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2003</v>
-      </c>
-      <c r="B26">
         <v>3.1711100000000001</v>
       </c>
-      <c r="C26">
-        <v>3.1711100000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2004</v>
-      </c>
-      <c r="B27">
         <v>6.3391700000000002</v>
       </c>
-      <c r="C27">
-        <v>6.3391700000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2005</v>
-      </c>
-      <c r="B28">
         <v>3.0285700000000002</v>
       </c>
-      <c r="C28">
-        <v>3.0285700000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2006</v>
-      </c>
-      <c r="B29">
         <v>5.3586400000000003</v>
       </c>
-      <c r="C29">
-        <v>5.3586400000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2007</v>
-      </c>
-      <c r="B30">
         <v>3.8971900000000002</v>
       </c>
-      <c r="C30">
-        <v>3.8971900000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2008</v>
-      </c>
-      <c r="B31">
         <v>4.2211600000000002</v>
       </c>
-      <c r="C31">
-        <v>4.2211600000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2009</v>
-      </c>
-      <c r="B32">
         <v>3.9105400000000001</v>
       </c>
-      <c r="C32">
-        <v>3.9105400000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2010</v>
-      </c>
-      <c r="B33">
         <v>8.9214599999999997</v>
       </c>
-      <c r="C33">
-        <v>8.9214599999999997</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2011</v>
-      </c>
-      <c r="B34">
         <v>2.51953</v>
       </c>
-      <c r="C34">
-        <v>2.51953</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2012</v>
-      </c>
-      <c r="B35">
         <v>4.6468299999999996</v>
       </c>
-      <c r="C35">
-        <v>4.6468299999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2013</v>
-      </c>
-      <c r="B36">
         <v>0.50890500000000005</v>
       </c>
-      <c r="C36">
-        <v>0.50890500000000005</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2014</v>
-      </c>
-      <c r="B37">
         <v>3.9941200000000001</v>
       </c>
-      <c r="C37">
-        <v>3.9941200000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2015</v>
-      </c>
-      <c r="B38">
         <v>6.60433</v>
       </c>
-      <c r="C38">
-        <v>6.60433</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2016</v>
-      </c>
-      <c r="B39">
         <v>75.171499999999995</v>
       </c>
-      <c r="C39">
-        <v>75.171499999999995</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2017</v>
-      </c>
-      <c r="B40">
         <v>20.059899999999999</v>
       </c>
-      <c r="C40">
-        <v>20.059899999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>2018</v>
-      </c>
-      <c r="B41">
         <v>6.2455999999999996</v>
-      </c>
-      <c r="C41">
-        <v>6.2455999999999996</v>
-      </c>
-    </row>
-    <row r="62" spans="41:41" x14ac:dyDescent="0.25">
-      <c r="AO62">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1979</v>
+        <v>4.6691630492362829E-2</v>
       </c>
       <c r="B2">
-        <v>10.4</v>
+        <v>0.12772012892412274</v>
       </c>
       <c r="C2">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1980</v>
-      </c>
-      <c r="B3">
-        <v>8.4</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1981</v>
-      </c>
-      <c r="B4">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1982</v>
-      </c>
-      <c r="B5">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="C5">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1983</v>
-      </c>
-      <c r="B6">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="C6">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1984</v>
-      </c>
-      <c r="B7">
-        <v>10.3</v>
-      </c>
-      <c r="C7">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1985</v>
-      </c>
-      <c r="B8">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1986</v>
-      </c>
-      <c r="B9">
-        <v>21.6</v>
-      </c>
-      <c r="C9">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1987</v>
-      </c>
-      <c r="B10">
-        <v>27.6</v>
-      </c>
-      <c r="C10">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1988</v>
-      </c>
-      <c r="B11">
-        <v>29.3</v>
-      </c>
-      <c r="C11">
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1989</v>
-      </c>
-      <c r="B12">
-        <v>27.5</v>
-      </c>
-      <c r="C12">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1990</v>
-      </c>
-      <c r="B13">
-        <v>25.532</v>
-      </c>
-      <c r="C13">
-        <v>4.6840000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1991</v>
-      </c>
-      <c r="B14">
-        <v>23.343330000000002</v>
-      </c>
-      <c r="C14">
-        <v>3.09735</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1992</v>
-      </c>
-      <c r="B15">
-        <v>20.988790000000002</v>
-      </c>
-      <c r="C15">
-        <v>2.9098700000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1993</v>
-      </c>
-      <c r="B16">
-        <v>22.9117</v>
-      </c>
-      <c r="C16">
-        <v>2.5055999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1994</v>
-      </c>
-      <c r="B17">
-        <v>20.639109999999999</v>
-      </c>
-      <c r="C17">
-        <v>2.9376099999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1995</v>
-      </c>
-      <c r="B18">
-        <v>18.238277005027399</v>
-      </c>
-      <c r="C18">
-        <v>2.6126100000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1996</v>
-      </c>
-      <c r="B19">
-        <v>15.320502605543201</v>
-      </c>
-      <c r="C19">
-        <v>2.18716</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1997</v>
-      </c>
-      <c r="B20">
-        <v>13.117830786668501</v>
-      </c>
-      <c r="C20">
-        <v>1.6315200000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1998</v>
-      </c>
-      <c r="B21">
-        <v>12.556547492511999</v>
-      </c>
-      <c r="C21">
-        <v>1.48726</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1999</v>
-      </c>
-      <c r="B22">
-        <v>11.737945834585901</v>
-      </c>
-      <c r="C22">
-        <v>1.98451</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2000</v>
-      </c>
-      <c r="B23">
-        <v>13.8452117838173</v>
-      </c>
-      <c r="C23">
-        <v>2.01939</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2001</v>
-      </c>
-      <c r="B24">
-        <v>12.6548875246433</v>
-      </c>
-      <c r="C24">
-        <v>1.7828999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2002</v>
-      </c>
-      <c r="B25">
-        <v>12.921144842025001</v>
-      </c>
-      <c r="C25">
-        <v>2.2431100000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2003</v>
-      </c>
-      <c r="B26">
-        <v>14.5193401736504</v>
-      </c>
-      <c r="C26">
-        <v>2.0602339999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2004</v>
-      </c>
-      <c r="B27">
-        <v>16.224240187409102</v>
-      </c>
-      <c r="C27">
-        <v>1.6564160000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2005</v>
-      </c>
-      <c r="B28">
-        <v>15.5068320699894</v>
-      </c>
-      <c r="C28">
-        <v>1.556249</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>2006</v>
-      </c>
-      <c r="B29">
-        <v>14.7971992285333</v>
-      </c>
-      <c r="C29">
-        <v>1.246329</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>2007</v>
-      </c>
-      <c r="B30">
-        <v>15.196407850112699</v>
-      </c>
-      <c r="C30">
-        <v>1.2353860000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>2008</v>
-      </c>
-      <c r="B31">
-        <v>13.712910758816401</v>
-      </c>
-      <c r="C31">
-        <v>1.1220570000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>2009</v>
-      </c>
-      <c r="B32">
-        <v>12.283396346141</v>
-      </c>
-      <c r="C32">
-        <v>1.056729</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>2010</v>
-      </c>
-      <c r="B33">
-        <v>11.345304725792699</v>
-      </c>
-      <c r="C33">
-        <v>1.004606413464</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>2011</v>
-      </c>
-      <c r="B34">
-        <v>12.082986601945199</v>
-      </c>
-      <c r="C34">
-        <v>1.1792639863204999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>2012</v>
-      </c>
-      <c r="B35">
-        <v>13.1901034522896</v>
-      </c>
-      <c r="C35">
-        <v>1.1018389988371999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>2013</v>
-      </c>
-      <c r="B36">
-        <v>13.0234404738802</v>
-      </c>
-      <c r="C36">
-        <v>1.0372264314243</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>2014</v>
-      </c>
-      <c r="B37">
-        <v>10.870098914022099</v>
-      </c>
-      <c r="C37">
-        <v>1.0253812582913</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>2015</v>
-      </c>
-      <c r="B38">
-        <v>10.204934118352099</v>
-      </c>
-      <c r="C38">
-        <v>1.0847270697564</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>2016</v>
-      </c>
-      <c r="B39">
-        <v>9.3370484481536309</v>
-      </c>
-      <c r="C39">
-        <v>1.3383677871965001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>2017</v>
-      </c>
-      <c r="B40">
-        <v>10.177195738843499</v>
-      </c>
-      <c r="C40">
-        <v>2.2798940528161</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>2018</v>
-      </c>
-      <c r="B41">
-        <v>10.199706999498</v>
-      </c>
-      <c r="C41">
-        <v>3.4294961723616302</v>
+        <v>0.36865873797750515</v>
+      </c>
+      <c r="D2">
+        <v>0.3541152884016216</v>
+      </c>
+      <c r="E2">
+        <v>6.4533382298702993E-2</v>
+      </c>
+      <c r="F2">
+        <v>3.8280831905684841E-2</v>
       </c>
     </row>
   </sheetData>
@@ -11053,6 +10299,1239 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
+        <v>0.56706853463412132</v>
+      </c>
+      <c r="B2" s="32">
+        <v>0.76595392819232544</v>
+      </c>
+      <c r="C2" s="32">
+        <v>1.1461127127972874</v>
+      </c>
+      <c r="D2" s="32">
+        <v>4.934379401402964</v>
+      </c>
+      <c r="E2" s="32">
+        <v>1.7215937091743347</v>
+      </c>
+      <c r="F2" s="32">
+        <v>2.7648917137989684</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="32">
+        <v>0.5118551074685358</v>
+      </c>
+      <c r="B3" s="32">
+        <v>0.64374349427395883</v>
+      </c>
+      <c r="C3" s="32">
+        <v>0.94920913841550247</v>
+      </c>
+      <c r="D3" s="32">
+        <v>4.5627597999571083</v>
+      </c>
+      <c r="E3" s="32">
+        <v>1.4738367649964228</v>
+      </c>
+      <c r="F3" s="32">
+        <v>2.2585956948884722</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="32">
+        <v>0.60070321603825283</v>
+      </c>
+      <c r="B4" s="32">
+        <v>0.81057191640544635</v>
+      </c>
+      <c r="C4" s="32">
+        <v>1.2126358659662135</v>
+      </c>
+      <c r="D4" s="32">
+        <v>5.2289114692687022</v>
+      </c>
+      <c r="E4" s="32">
+        <v>1.8223389387355855</v>
+      </c>
+      <c r="F4" s="32">
+        <v>2.9248385935857995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>0.57861784517201864</v>
+      </c>
+      <c r="B5" s="32">
+        <v>0.76168774283809959</v>
+      </c>
+      <c r="C5" s="32">
+        <v>1.1338744362134994</v>
+      </c>
+      <c r="D5" s="32">
+        <v>5.0802636286903606</v>
+      </c>
+      <c r="E5" s="32">
+        <v>1.7232361610644209</v>
+      </c>
+      <c r="F5" s="32">
+        <v>2.7223201860216006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <v>0.56496132256845399</v>
+      </c>
+      <c r="B6" s="32">
+        <v>0.75532385640801092</v>
+      </c>
+      <c r="C6" s="32">
+        <v>1.127912771529987</v>
+      </c>
+      <c r="D6" s="32">
+        <v>4.933826678744774</v>
+      </c>
+      <c r="E6" s="32">
+        <v>1.7021016440181187</v>
+      </c>
+      <c r="F6" s="32">
+        <v>2.715873726730655</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
+        <v>0.7196508078913908</v>
+      </c>
+      <c r="B7" s="32">
+        <v>0.83223261463866649</v>
+      </c>
+      <c r="C7" s="32">
+        <v>1.2040814698531526</v>
+      </c>
+      <c r="D7" s="32">
+        <v>6.5815187269617148</v>
+      </c>
+      <c r="E7" s="32">
+        <v>1.9496109933671253</v>
+      </c>
+      <c r="F7" s="32">
+        <v>2.8129053872879508</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="32">
+        <v>0.68322968841096776</v>
+      </c>
+      <c r="B8" s="32">
+        <v>0.9455101231839903</v>
+      </c>
+      <c r="C8" s="32">
+        <v>1.4214627697150233</v>
+      </c>
+      <c r="D8" s="32">
+        <v>5.8934049706057294</v>
+      </c>
+      <c r="E8" s="32">
+        <v>2.1123649170061016</v>
+      </c>
+      <c r="F8" s="32">
+        <v>3.4440275310781874</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="32">
+        <v>1.463494198714683</v>
+      </c>
+      <c r="B9" s="32">
+        <v>1.723979474628994</v>
+      </c>
+      <c r="C9" s="32">
+        <v>2.5051243107263192</v>
+      </c>
+      <c r="D9" s="32">
+        <v>13.312238017159961</v>
+      </c>
+      <c r="E9" s="32">
+        <v>4.0178168295616317</v>
+      </c>
+      <c r="F9" s="32">
+        <v>5.8773471692084138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="32">
+        <v>1.752043183643522</v>
+      </c>
+      <c r="B10" s="32">
+        <v>2.1478857542548924</v>
+      </c>
+      <c r="C10" s="32">
+        <v>3.1494900160232864</v>
+      </c>
+      <c r="D10" s="32">
+        <v>15.745029371007801</v>
+      </c>
+      <c r="E10" s="32">
+        <v>4.9512983155120862</v>
+      </c>
+      <c r="F10" s="32">
+        <v>7.4542533595584146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="32">
+        <v>1.9304186267935801</v>
+      </c>
+      <c r="B11" s="32">
+        <v>2.3130170299751081</v>
+      </c>
+      <c r="C11" s="32">
+        <v>3.3742390768266111</v>
+      </c>
+      <c r="D11" s="32">
+        <v>17.470361675463046</v>
+      </c>
+      <c r="E11" s="32">
+        <v>5.365311444633968</v>
+      </c>
+      <c r="F11" s="32">
+        <v>7.9466521463076889</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="32">
+        <v>1.72709066305445</v>
+      </c>
+      <c r="B12" s="32">
+        <v>2.1314339171100798</v>
+      </c>
+      <c r="C12" s="32">
+        <v>3.1299571321934891</v>
+      </c>
+      <c r="D12" s="32">
+        <v>15.488488347273931</v>
+      </c>
+      <c r="E12" s="32">
+        <v>4.9045668781029494</v>
+      </c>
+      <c r="F12" s="32">
+        <v>7.4184630622651024</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="32">
+        <v>1.4605382894641181</v>
+      </c>
+      <c r="B13" s="32">
+        <v>1.9122840550108282</v>
+      </c>
+      <c r="C13" s="32">
+        <v>2.8435597458200292</v>
+      </c>
+      <c r="D13" s="32">
+        <v>12.847184457296798</v>
+      </c>
+      <c r="E13" s="32">
+        <v>4.3323436501323496</v>
+      </c>
+      <c r="F13" s="32">
+        <v>6.820089802275878</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="32">
+        <v>1.20902</v>
+      </c>
+      <c r="B14" s="32">
+        <v>2.1900900000000001</v>
+      </c>
+      <c r="C14" s="32">
+        <v>1.9314800000000001</v>
+      </c>
+      <c r="D14" s="32">
+        <v>11.177910000000002</v>
+      </c>
+      <c r="E14" s="32">
+        <v>4.0690799999999996</v>
+      </c>
+      <c r="F14" s="32">
+        <v>5.8691300000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="32">
+        <v>0.61258999999999997</v>
+      </c>
+      <c r="B15" s="32">
+        <v>1.5531300000000001</v>
+      </c>
+      <c r="C15" s="32">
+        <v>2.2212200000000002</v>
+      </c>
+      <c r="D15" s="32">
+        <v>10.35492</v>
+      </c>
+      <c r="E15" s="32">
+        <v>4.4080000000000004</v>
+      </c>
+      <c r="F15" s="32">
+        <v>4.7500299999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="32">
+        <v>0.66908999999999996</v>
+      </c>
+      <c r="B16" s="32">
+        <v>2.0775100000000002</v>
+      </c>
+      <c r="C16" s="32">
+        <v>0.73952000000000007</v>
+      </c>
+      <c r="D16" s="32">
+        <v>11.95491</v>
+      </c>
+      <c r="E16" s="32">
+        <v>4.6197900000000001</v>
+      </c>
+      <c r="F16" s="32">
+        <v>5.3564799999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="32">
+        <v>0.69407999999999992</v>
+      </c>
+      <c r="B17" s="32">
+        <v>1.7272100000000001</v>
+      </c>
+      <c r="C17" s="32">
+        <v>0.53907000000000005</v>
+      </c>
+      <c r="D17" s="32">
+        <v>9.3765900000000002</v>
+      </c>
+      <c r="E17" s="32">
+        <v>4.4932800000000004</v>
+      </c>
+      <c r="F17" s="32">
+        <v>6.7497299999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="32">
+        <v>0.92962000000000011</v>
+      </c>
+      <c r="B18" s="32">
+        <v>1.1190599999999999</v>
+      </c>
+      <c r="C18" s="32">
+        <v>1.74685</v>
+      </c>
+      <c r="D18" s="32">
+        <v>7.672950000000001</v>
+      </c>
+      <c r="E18" s="32">
+        <v>3.8716500000000003</v>
+      </c>
+      <c r="F18" s="32">
+        <v>5.3515400000000009</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="32">
+        <v>0.64839999999999998</v>
+      </c>
+      <c r="B19" s="32">
+        <v>0.76422000000000001</v>
+      </c>
+      <c r="C19" s="32">
+        <v>1.6492600000000002</v>
+      </c>
+      <c r="D19" s="32">
+        <v>6.772549999999999</v>
+      </c>
+      <c r="E19" s="32">
+        <v>2.899</v>
+      </c>
+      <c r="F19" s="32">
+        <v>4.6593999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="32">
+        <v>0.55162</v>
+      </c>
+      <c r="B20" s="32">
+        <v>0.78125</v>
+      </c>
+      <c r="C20" s="32">
+        <v>1.37432</v>
+      </c>
+      <c r="D20" s="32">
+        <v>6.2343699999999993</v>
+      </c>
+      <c r="E20" s="32">
+        <v>1.93004</v>
+      </c>
+      <c r="F20" s="32">
+        <v>3.7354900000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="32">
+        <v>0.56286999999999998</v>
+      </c>
+      <c r="B21" s="32">
+        <v>0.53525999999999996</v>
+      </c>
+      <c r="C21" s="32">
+        <v>1.4321699999999999</v>
+      </c>
+      <c r="D21" s="32">
+        <v>5.9215400000000011</v>
+      </c>
+      <c r="E21" s="32">
+        <v>1.9555199999999999</v>
+      </c>
+      <c r="F21" s="32">
+        <v>3.4668400000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="32">
+        <v>0.67503999999999997</v>
+      </c>
+      <c r="B22" s="32">
+        <v>0.68259999999999998</v>
+      </c>
+      <c r="C22" s="32">
+        <v>1.4880100000000003</v>
+      </c>
+      <c r="D22" s="32">
+        <v>5.87439</v>
+      </c>
+      <c r="E22" s="32">
+        <v>1.70851</v>
+      </c>
+      <c r="F22" s="32">
+        <v>3.1585100000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="32">
+        <v>0.7419</v>
+      </c>
+      <c r="B23" s="32">
+        <v>1.0486900000000001</v>
+      </c>
+      <c r="C23" s="32">
+        <v>1.5868899999999999</v>
+      </c>
+      <c r="D23" s="32">
+        <v>6.1732700000000005</v>
+      </c>
+      <c r="E23" s="32">
+        <v>2.0662800000000003</v>
+      </c>
+      <c r="F23" s="32">
+        <v>3.9532399999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="32">
+        <v>0.86382999999999999</v>
+      </c>
+      <c r="B24" s="32">
+        <v>1.0740699999999999</v>
+      </c>
+      <c r="C24" s="32">
+        <v>1.5880500000000002</v>
+      </c>
+      <c r="D24" s="32">
+        <v>5.5180600000000002</v>
+      </c>
+      <c r="E24" s="32">
+        <v>1.7368400000000002</v>
+      </c>
+      <c r="F24" s="32">
+        <v>3.2837200000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="32">
+        <v>1.14375</v>
+      </c>
+      <c r="B25" s="32">
+        <v>1.1184999999999998</v>
+      </c>
+      <c r="C25" s="32">
+        <v>1.86494</v>
+      </c>
+      <c r="D25" s="32">
+        <v>6.1799900000000001</v>
+      </c>
+      <c r="E25" s="32">
+        <v>1.54989</v>
+      </c>
+      <c r="F25" s="32">
+        <v>2.89107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="32">
+        <v>1.0115610000000002</v>
+      </c>
+      <c r="B26" s="32">
+        <v>1.1178700000000001</v>
+      </c>
+      <c r="C26" s="32">
+        <v>2.1182970000000001</v>
+      </c>
+      <c r="D26" s="32">
+        <v>6.993661000000011</v>
+      </c>
+      <c r="E26" s="32">
+        <v>1.8223059999999998</v>
+      </c>
+      <c r="F26" s="32">
+        <v>3.3473120000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="32">
+        <v>1.0407500000000001</v>
+      </c>
+      <c r="B27" s="32">
+        <v>0.95535899999999996</v>
+      </c>
+      <c r="C27" s="32">
+        <v>2.1731009999999999</v>
+      </c>
+      <c r="D27" s="32">
+        <v>7.3096900000000007</v>
+      </c>
+      <c r="E27" s="32">
+        <v>2.2409020000000002</v>
+      </c>
+      <c r="F27" s="32">
+        <v>3.8005580000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="32">
+        <v>1.0700319999999999</v>
+      </c>
+      <c r="B28" s="32">
+        <v>1.480958</v>
+      </c>
+      <c r="C28" s="32">
+        <v>1.9298269999999997</v>
+      </c>
+      <c r="D28" s="32">
+        <v>6.7055759999999891</v>
+      </c>
+      <c r="E28" s="32">
+        <v>1.823976</v>
+      </c>
+      <c r="F28" s="32">
+        <v>3.5746449999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="32">
+        <v>1.0783579999999999</v>
+      </c>
+      <c r="B29" s="32">
+        <v>1.1505530000000002</v>
+      </c>
+      <c r="C29" s="32">
+        <v>2.1508000000000003</v>
+      </c>
+      <c r="D29" s="32">
+        <v>5.9206129999999995</v>
+      </c>
+      <c r="E29" s="32">
+        <v>1.8891300000000002</v>
+      </c>
+      <c r="F29" s="32">
+        <v>3.361704</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="32">
+        <v>1.1816469999999999</v>
+      </c>
+      <c r="B30" s="32">
+        <v>1.1685910000000002</v>
+      </c>
+      <c r="C30" s="32">
+        <v>2.1013280000000001</v>
+      </c>
+      <c r="D30" s="32">
+        <v>6.0042730000000013</v>
+      </c>
+      <c r="E30" s="32">
+        <v>2.0736110000000001</v>
+      </c>
+      <c r="F30" s="32">
+        <v>3.428741</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="32">
+        <v>1.140998</v>
+      </c>
+      <c r="B31" s="32">
+        <v>0.89897399999999994</v>
+      </c>
+      <c r="C31" s="32">
+        <v>1.6792959999999999</v>
+      </c>
+      <c r="D31" s="32">
+        <v>5.4950320000000001</v>
+      </c>
+      <c r="E31" s="32">
+        <v>2.0161920000000002</v>
+      </c>
+      <c r="F31" s="32">
+        <v>3.3212199999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="32">
+        <v>0.916018</v>
+      </c>
+      <c r="B32" s="32">
+        <v>1.0997750000000002</v>
+      </c>
+      <c r="C32" s="32">
+        <v>1.422695</v>
+      </c>
+      <c r="D32" s="32">
+        <v>4.9672190000000001</v>
+      </c>
+      <c r="E32" s="32">
+        <v>1.8314849999999998</v>
+      </c>
+      <c r="F32" s="32">
+        <v>2.8248339999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="32">
+        <v>0.75416021215880003</v>
+      </c>
+      <c r="B33" s="32">
+        <v>1.0481037166614</v>
+      </c>
+      <c r="C33" s="32">
+        <v>1.3542938055945</v>
+      </c>
+      <c r="D33" s="32">
+        <v>4.5101234593954995</v>
+      </c>
+      <c r="E33" s="32">
+        <v>1.5787251126747999</v>
+      </c>
+      <c r="F33" s="32">
+        <v>2.6913501691308004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="32">
+        <v>0.70768533684400003</v>
+      </c>
+      <c r="B34" s="32">
+        <v>1.0276654679888</v>
+      </c>
+      <c r="C34" s="32">
+        <v>1.3973503051538001</v>
+      </c>
+      <c r="D34" s="32">
+        <v>4.9205110890368999</v>
+      </c>
+      <c r="E34" s="32">
+        <v>1.9032203478823</v>
+      </c>
+      <c r="F34" s="32">
+        <v>3.0364416616812</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="32">
+        <v>0.74461771357649997</v>
+      </c>
+      <c r="B35" s="32">
+        <v>1.2052987019811001</v>
+      </c>
+      <c r="C35" s="32">
+        <v>1.3531629751415999</v>
+      </c>
+      <c r="D35" s="32">
+        <v>5.3302838770981911</v>
+      </c>
+      <c r="E35" s="32">
+        <v>2.0334334014981996</v>
+      </c>
+      <c r="F35" s="32">
+        <v>3.2059891770808999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="32">
+        <v>0.63465581828639994</v>
+      </c>
+      <c r="B36" s="32">
+        <v>1.0645311173309999</v>
+      </c>
+      <c r="C36" s="32">
+        <v>1.3844697979623</v>
+      </c>
+      <c r="D36" s="32">
+        <v>5.2082066386871997</v>
+      </c>
+      <c r="E36" s="32">
+        <v>2.1076726269653001</v>
+      </c>
+      <c r="F36" s="32">
+        <v>3.2471872931229999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="32">
+        <v>0.31293048738000001</v>
+      </c>
+      <c r="B37" s="32">
+        <v>0.82090823418470005</v>
+      </c>
+      <c r="C37" s="32">
+        <v>1.2019135006866</v>
+      </c>
+      <c r="D37" s="32">
+        <v>4.7566803862539997</v>
+      </c>
+      <c r="E37" s="32">
+        <v>1.6702062545069998</v>
+      </c>
+      <c r="F37" s="32">
+        <v>2.822162336351</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="32">
+        <v>0.21039000067089997</v>
+      </c>
+      <c r="B38" s="32">
+        <v>0.43067203148989996</v>
+      </c>
+      <c r="C38" s="32">
+        <v>1.0139265986634001</v>
+      </c>
+      <c r="D38" s="32">
+        <v>4.6456995525671001</v>
+      </c>
+      <c r="E38" s="32">
+        <v>1.8409850388593001</v>
+      </c>
+      <c r="F38" s="32">
+        <v>2.8296751491737999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="32">
+        <v>0.53190304368810004</v>
+      </c>
+      <c r="B39" s="32">
+        <v>0.34917000969959999</v>
+      </c>
+      <c r="C39" s="32">
+        <v>1.0583306849187</v>
+      </c>
+      <c r="D39" s="32">
+        <v>4.1994769794157998</v>
+      </c>
+      <c r="E39" s="32">
+        <v>1.6564156912200001</v>
+      </c>
+      <c r="F39" s="32">
+        <v>2.4636165809348998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="32">
+        <v>1.1586105415015999</v>
+      </c>
+      <c r="B40" s="32">
+        <v>0.59006990085000011</v>
+      </c>
+      <c r="C40" s="32">
+        <v>1.1814223483342001</v>
+      </c>
+      <c r="D40" s="32">
+        <v>4.8433747021564999</v>
+      </c>
+      <c r="E40" s="32">
+        <v>1.6982683437830002</v>
+      </c>
+      <c r="F40" s="32">
+        <v>2.7982629160748997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="32">
+        <v>1.573968902057</v>
+      </c>
+      <c r="B41" s="32">
+        <v>0.64546162485109992</v>
+      </c>
+      <c r="C41" s="32">
+        <v>1.4008347950712992</v>
+      </c>
+      <c r="D41" s="32">
+        <v>5.8233072909484003</v>
+      </c>
+      <c r="E41" s="32">
+        <v>1.8272960632783</v>
+      </c>
+      <c r="F41" s="32">
+        <v>2.9941775262591999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2">
+        <v>4.3557731816054697E-3</v>
+      </c>
+      <c r="C2">
+        <v>4.1754783665450712E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.12303968930267978</v>
+      </c>
+      <c r="E2">
+        <v>0.17023797738832738</v>
+      </c>
+      <c r="F2">
+        <v>0.15885158540438304</v>
+      </c>
+      <c r="G2">
+        <v>0.11169825819416687</v>
+      </c>
+      <c r="H2">
+        <v>7.36412602457161E-2</v>
+      </c>
+      <c r="I2">
+        <v>4.6283280147181763E-2</v>
+      </c>
+      <c r="J2">
+        <v>3.639346528551031E-2</v>
+      </c>
+      <c r="K2">
+        <v>2.5479883802611548E-2</v>
+      </c>
+      <c r="L2">
+        <v>1.8867910317620289E-2</v>
+      </c>
+      <c r="M2">
+        <v>1.510360359505955E-2</v>
+      </c>
+      <c r="N2">
+        <v>1.4156750540760064E-2</v>
+      </c>
+      <c r="O2">
+        <v>1.2517390786867441E-2</v>
+      </c>
+      <c r="P2">
+        <v>1.0381800394444911E-2</v>
+      </c>
+      <c r="Q2">
+        <v>9.4091409262688878E-3</v>
+      </c>
+      <c r="R2">
+        <v>6.184506325945467E-3</v>
+      </c>
+      <c r="S2">
+        <v>5.3590070737419629E-3</v>
+      </c>
+      <c r="T2">
+        <v>6.6909622790304029E-3</v>
+      </c>
+      <c r="U2">
+        <v>5.8610807193160896E-3</v>
+      </c>
+      <c r="V2">
+        <v>5.4963251925338732E-3</v>
+      </c>
+      <c r="W2">
+        <v>4.7046881988527202E-3</v>
+      </c>
+      <c r="X2">
+        <v>3.8977743757753931E-3</v>
+      </c>
+      <c r="Y2">
+        <v>3.8711649051295458E-3</v>
+      </c>
+      <c r="Z2">
+        <v>5.2271702043151218E-3</v>
+      </c>
+      <c r="AA2">
+        <v>3.5521804377124022E-3</v>
+      </c>
+      <c r="AB2">
+        <v>3.6001896909224687E-3</v>
+      </c>
+      <c r="AC2">
+        <v>4.1268564457153951E-3</v>
+      </c>
+      <c r="AD2">
+        <v>4.315662662422939E-3</v>
+      </c>
+      <c r="AE2">
+        <v>6.493987830993217E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3">
+        <v>2.4815418179572153E-3</v>
+      </c>
+      <c r="C3">
+        <v>1.8150841629395897E-2</v>
+      </c>
+      <c r="D3">
+        <v>5.5747308609011281E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.10747654437326125</v>
+      </c>
+      <c r="F3">
+        <v>0.13519789870106549</v>
+      </c>
+      <c r="G3">
+        <v>0.12168091627942444</v>
+      </c>
+      <c r="H3">
+        <v>8.1138280149756048E-2</v>
+      </c>
+      <c r="I3">
+        <v>6.3516896731352371E-2</v>
+      </c>
+      <c r="J3">
+        <v>5.1738887618923583E-2</v>
+      </c>
+      <c r="K3">
+        <v>3.962854885248198E-2</v>
+      </c>
+      <c r="L3">
+        <v>2.8482094871486428E-2</v>
+      </c>
+      <c r="M3">
+        <v>3.7895672934557895E-2</v>
+      </c>
+      <c r="N3">
+        <v>2.9159774036970509E-2</v>
+      </c>
+      <c r="O3">
+        <v>2.8191416981484804E-2</v>
+      </c>
+      <c r="P3">
+        <v>2.6379312866675428E-2</v>
+      </c>
+      <c r="Q3">
+        <v>1.9808405299671015E-2</v>
+      </c>
+      <c r="R3">
+        <v>2.1024624842119529E-2</v>
+      </c>
+      <c r="S3">
+        <v>1.2956908348928766E-2</v>
+      </c>
+      <c r="T3">
+        <v>1.1857416938422764E-2</v>
+      </c>
+      <c r="U3">
+        <v>9.9688150738798734E-3</v>
+      </c>
+      <c r="V3">
+        <v>5.2350877192971308E-3</v>
+      </c>
+      <c r="W3">
+        <v>1.0702934988646284E-2</v>
+      </c>
+      <c r="X3">
+        <v>1.0142009560240708E-2</v>
+      </c>
+      <c r="Y3">
+        <v>1.0162394860752443E-2</v>
+      </c>
+      <c r="Z3">
+        <v>4.2418167299620836E-3</v>
+      </c>
+      <c r="AA3">
+        <v>4.8493601232404938E-3</v>
+      </c>
+      <c r="AB3">
+        <v>5.4243153521983138E-3</v>
+      </c>
+      <c r="AC3">
+        <v>3.666451309479974E-3</v>
+      </c>
+      <c r="AD3">
+        <v>4.4917421253122163E-3</v>
+      </c>
+      <c r="AE3">
+        <v>3.8601780274043637E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4">
+        <v>1.6601183050664636E-3</v>
+      </c>
+      <c r="C4">
+        <v>1.0982678751052221E-2</v>
+      </c>
+      <c r="D4">
+        <v>2.8518133097095298E-2</v>
+      </c>
+      <c r="E4">
+        <v>7.8869303169007726E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.10668974864015558</v>
+      </c>
+      <c r="G4">
+        <v>0.10949844090419208</v>
+      </c>
+      <c r="H4">
+        <v>9.2190463078216114E-2</v>
+      </c>
+      <c r="I4">
+        <v>7.0783455651711652E-2</v>
+      </c>
+      <c r="J4">
+        <v>6.2253237163515621E-2</v>
+      </c>
+      <c r="K4">
+        <v>5.9113917116188096E-2</v>
+      </c>
+      <c r="L4">
+        <v>5.0063979295548136E-2</v>
+      </c>
+      <c r="M4">
+        <v>4.3043908834068209E-2</v>
+      </c>
+      <c r="N4">
+        <v>3.4228961278893966E-2</v>
+      </c>
+      <c r="O4">
+        <v>2.9174237545620915E-2</v>
+      </c>
+      <c r="P4">
+        <v>2.3421672534823381E-2</v>
+      </c>
+      <c r="Q4">
+        <v>2.4279626858457262E-2</v>
+      </c>
+      <c r="R4">
+        <v>1.8117907793622021E-2</v>
+      </c>
+      <c r="S4">
+        <v>1.3436653733596888E-2</v>
+      </c>
+      <c r="T4">
+        <v>1.5667380995311474E-2</v>
+      </c>
+      <c r="U4">
+        <v>1.2891340933049542E-2</v>
+      </c>
+      <c r="V4">
+        <v>8.8139856718907148E-3</v>
+      </c>
+      <c r="W4">
+        <v>1.2414375010697441E-2</v>
+      </c>
+      <c r="X4">
+        <v>8.9998130766681464E-3</v>
+      </c>
+      <c r="Y4">
+        <v>6.8387047458654598E-3</v>
+      </c>
+      <c r="Z4">
+        <v>7.3376209240679884E-3</v>
+      </c>
+      <c r="AA4">
+        <v>9.0232521476115088E-3</v>
+      </c>
+      <c r="AB4">
+        <v>5.695549816805842E-3</v>
+      </c>
+      <c r="AC4">
+        <v>5.0469833819998828E-3</v>
+      </c>
+      <c r="AD4">
+        <v>5.9990650627871536E-3</v>
+      </c>
+      <c r="AE4">
+        <v>4.4945484482413145E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -11200,7 +11679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -11295,124 +11774,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2">
-        <v>0.1</v>
-      </c>
-      <c r="C2">
-        <v>0.1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3">
-        <v>7.9500000000000001E-2</v>
-      </c>
-      <c r="C3">
-        <v>9.7500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>16.5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3">
-        <v>1.2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated to include length bins
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -1,33 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Sablefish_ApportionmentStrategies\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curryc2/Documents/NOAA/2018/Sablefish MSE/Sablefish_ApportionmentStrategies/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DF4132-09A3-0F46-9FBF-032CEDFDA159}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="22080" tabRatio="767"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Sim" sheetId="4" r:id="rId2"/>
-    <sheet name="Growth" sheetId="2" r:id="rId3"/>
-    <sheet name="Maturity" sheetId="3" r:id="rId4"/>
-    <sheet name="Mortality" sheetId="5" r:id="rId5"/>
-    <sheet name="Recruitment" sheetId="6" r:id="rId6"/>
-    <sheet name="Catchability_SAFE" sheetId="7" r:id="rId7"/>
-    <sheet name="SurveySelectivity" sheetId="8" r:id="rId8"/>
-    <sheet name="SurveySelexType" sheetId="11" r:id="rId9"/>
-    <sheet name="qSurvey" sheetId="12" r:id="rId10"/>
-    <sheet name="FisherySelectivity" sheetId="9" r:id="rId11"/>
-    <sheet name="FisherySelexType" sheetId="14" r:id="rId12"/>
-    <sheet name="qFishery" sheetId="15" r:id="rId13"/>
-    <sheet name="Movement" sheetId="16" r:id="rId14"/>
+    <sheet name="Length_Bins" sheetId="18" r:id="rId3"/>
+    <sheet name="Growth" sheetId="2" r:id="rId4"/>
+    <sheet name="Maturity" sheetId="3" r:id="rId5"/>
+    <sheet name="Mortality" sheetId="5" r:id="rId6"/>
+    <sheet name="Recruitment" sheetId="6" r:id="rId7"/>
+    <sheet name="Catchability_SAFE" sheetId="7" r:id="rId8"/>
+    <sheet name="SurveySelectivity" sheetId="8" r:id="rId9"/>
+    <sheet name="SurveySelexType" sheetId="11" r:id="rId10"/>
+    <sheet name="qSurvey" sheetId="12" r:id="rId11"/>
+    <sheet name="FisherySelectivity" sheetId="9" r:id="rId12"/>
+    <sheet name="FisherySelexType" sheetId="14" r:id="rId13"/>
+    <sheet name="qFishery" sheetId="15" r:id="rId14"/>
+    <sheet name="Movement" sheetId="16" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -37,12 +39,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Curry Cunningham</author>
   </authors>
   <commentList>
-    <comment ref="C14" authorId="0" shapeId="0">
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -312,8 +314,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1025,16 +1027,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1056,7 +1058,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1067,7 +1069,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1078,7 +1080,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1089,7 +1091,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1100,7 +1102,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -1111,7 +1113,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1122,7 +1124,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -1133,7 +1135,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -1155,159 +1157,40 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C13"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="19">
-        <v>1</v>
-      </c>
-      <c r="C8" s="18">
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="19">
-        <v>2</v>
-      </c>
-      <c r="C9" s="18">
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="19">
-        <v>3</v>
-      </c>
-      <c r="C10" s="18">
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="19">
-        <v>4</v>
-      </c>
-      <c r="C11" s="18">
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="19">
-        <v>5</v>
-      </c>
-      <c r="C12" s="18">
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="19">
-        <v>6</v>
-      </c>
-      <c r="C13" s="18">
-        <v>1.62</v>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1322,19 +1205,186 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:4" s="6" customFormat="1">
+      <c r="A1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="19">
+        <v>1</v>
+      </c>
+      <c r="C8" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="19">
+        <v>2</v>
+      </c>
+      <c r="C9" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="19">
+        <v>3</v>
+      </c>
+      <c r="C10" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="19">
+        <v>4</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="19">
+        <v>5</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="19">
+        <v>6</v>
+      </c>
+      <c r="C13" s="18">
+        <v>1.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -1354,7 +1404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="16" t="s">
         <v>66</v>
       </c>
@@ -1371,7 +1421,7 @@
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="16" t="s">
         <v>66</v>
       </c>
@@ -1388,7 +1438,7 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="16" t="s">
         <v>66</v>
       </c>
@@ -1401,7 +1451,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="16" t="s">
         <v>66</v>
       </c>
@@ -1418,7 +1468,7 @@
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="16" t="s">
         <v>66</v>
       </c>
@@ -1435,7 +1485,7 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="16" t="s">
         <v>66</v>
       </c>
@@ -1448,7 +1498,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="16" t="s">
         <v>66</v>
       </c>
@@ -1465,7 +1515,7 @@
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="16" t="s">
         <v>66</v>
       </c>
@@ -1482,7 +1532,7 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="16" t="s">
         <v>66</v>
       </c>
@@ -1495,7 +1545,7 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="16" t="s">
         <v>66</v>
       </c>
@@ -1512,7 +1562,7 @@
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="16" t="s">
         <v>66</v>
       </c>
@@ -1529,7 +1579,7 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="16" t="s">
         <v>66</v>
       </c>
@@ -1542,7 +1592,7 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="16" t="s">
         <v>66</v>
       </c>
@@ -1559,7 +1609,7 @@
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="16" t="s">
         <v>66</v>
       </c>
@@ -1576,7 +1626,7 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="16" t="s">
         <v>66</v>
       </c>
@@ -1589,7 +1639,7 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="16" t="s">
         <v>66</v>
       </c>
@@ -1606,7 +1656,7 @@
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="16" t="s">
         <v>66</v>
       </c>
@@ -1623,7 +1673,7 @@
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="16" t="s">
         <v>66</v>
       </c>
@@ -1636,7 +1686,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
         <v>67</v>
       </c>
@@ -1653,7 +1703,7 @@
         <v>0.83233751308500004</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
         <v>67</v>
       </c>
@@ -1670,7 +1720,7 @@
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
         <v>67</v>
       </c>
@@ -1683,7 +1733,7 @@
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
         <v>67</v>
       </c>
@@ -1700,7 +1750,7 @@
         <v>0.83233751308500004</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
         <v>67</v>
       </c>
@@ -1717,7 +1767,7 @@
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
         <v>67</v>
       </c>
@@ -1730,7 +1780,7 @@
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="11" t="s">
         <v>67</v>
       </c>
@@ -1747,7 +1797,7 @@
         <v>0.83233751308500004</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="11" t="s">
         <v>67</v>
       </c>
@@ -1764,7 +1814,7 @@
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
         <v>67</v>
       </c>
@@ -1777,7 +1827,7 @@
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
         <v>67</v>
       </c>
@@ -1794,7 +1844,7 @@
         <v>1.1762722908800001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
         <v>67</v>
       </c>
@@ -1811,7 +1861,7 @@
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
         <v>67</v>
       </c>
@@ -1824,7 +1874,7 @@
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
         <v>67</v>
       </c>
@@ -1841,7 +1891,7 @@
         <v>1.29701630606</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="11" t="s">
         <v>67</v>
       </c>
@@ -1858,7 +1908,7 @@
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="11" t="s">
         <v>67</v>
       </c>
@@ -1871,7 +1921,7 @@
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="11" t="s">
         <v>67</v>
       </c>
@@ -1888,7 +1938,7 @@
         <v>1.29701630606</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="11" t="s">
         <v>67</v>
       </c>
@@ -1905,7 +1955,7 @@
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="11" t="s">
         <v>67</v>
       </c>
@@ -1918,7 +1968,7 @@
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="11" t="s">
         <v>57</v>
       </c>
@@ -1934,7 +1984,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="11" t="s">
         <v>57</v>
       </c>
@@ -1954,7 +2004,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="11" t="s">
         <v>57</v>
       </c>
@@ -1974,7 +2024,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="11" t="s">
         <v>57</v>
       </c>
@@ -1990,7 +2040,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="11" t="s">
         <v>57</v>
       </c>
@@ -2010,7 +2060,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="11" t="s">
         <v>57</v>
       </c>
@@ -2030,7 +2080,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="11" t="s">
         <v>57</v>
       </c>
@@ -2046,7 +2096,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="11" t="s">
         <v>57</v>
       </c>
@@ -2066,7 +2116,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="11" t="s">
         <v>57</v>
       </c>
@@ -2086,7 +2136,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="11" t="s">
         <v>57</v>
       </c>
@@ -2102,7 +2152,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="11" t="s">
         <v>57</v>
       </c>
@@ -2122,7 +2172,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="11" t="s">
         <v>57</v>
       </c>
@@ -2142,7 +2192,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="11" t="s">
         <v>57</v>
       </c>
@@ -2158,7 +2208,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="11" t="s">
         <v>57</v>
       </c>
@@ -2178,7 +2228,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="11" t="s">
         <v>57</v>
       </c>
@@ -2198,7 +2248,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="11" t="s">
         <v>57</v>
       </c>
@@ -2214,7 +2264,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="11" t="s">
         <v>57</v>
       </c>
@@ -2234,7 +2284,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="11" t="s">
         <v>57</v>
       </c>
@@ -2254,7 +2304,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="11" t="s">
         <v>59</v>
       </c>
@@ -2271,7 +2321,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="11" t="s">
         <v>59</v>
       </c>
@@ -2288,7 +2338,7 @@
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="11" t="s">
         <v>59</v>
       </c>
@@ -2301,7 +2351,7 @@
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="11" t="s">
         <v>59</v>
       </c>
@@ -2318,7 +2368,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="11" t="s">
         <v>59</v>
       </c>
@@ -2335,7 +2385,7 @@
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="11" t="s">
         <v>59</v>
       </c>
@@ -2348,7 +2398,7 @@
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="11" t="s">
         <v>59</v>
       </c>
@@ -2365,7 +2415,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="11" t="s">
         <v>59</v>
       </c>
@@ -2382,7 +2432,7 @@
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="11" t="s">
         <v>59</v>
       </c>
@@ -2395,7 +2445,7 @@
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="11" t="s">
         <v>59</v>
       </c>
@@ -2412,7 +2462,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="11" t="s">
         <v>59</v>
       </c>
@@ -2429,7 +2479,7 @@
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="11" t="s">
         <v>59</v>
       </c>
@@ -2442,7 +2492,7 @@
       <c r="D67" s="15"/>
       <c r="E67" s="15"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="11" t="s">
         <v>59</v>
       </c>
@@ -2459,7 +2509,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="11" t="s">
         <v>59</v>
       </c>
@@ -2476,7 +2526,7 @@
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="11" t="s">
         <v>59</v>
       </c>
@@ -2489,7 +2539,7 @@
       <c r="D70" s="15"/>
       <c r="E70" s="15"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="11" t="s">
         <v>59</v>
       </c>
@@ -2506,7 +2556,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="11" t="s">
         <v>59</v>
       </c>
@@ -2523,7 +2573,7 @@
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="11" t="s">
         <v>59</v>
       </c>
@@ -2607,20 +2657,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -2628,7 +2678,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="28" t="s">
         <v>66</v>
       </c>
@@ -2636,7 +2686,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="28" t="s">
         <v>67</v>
       </c>
@@ -2644,7 +2694,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="28" t="s">
         <v>57</v>
       </c>
@@ -2652,7 +2702,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="28" t="s">
         <v>59</v>
       </c>
@@ -2682,20 +2732,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="21.375" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -2709,7 +2759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="16" t="s">
         <v>66</v>
       </c>
@@ -2721,7 +2771,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="16" t="s">
         <v>66</v>
       </c>
@@ -2733,7 +2783,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="16" t="s">
         <v>66</v>
       </c>
@@ -2745,7 +2795,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="16" t="s">
         <v>66</v>
       </c>
@@ -2756,7 +2806,7 @@
         <v>1.1852290194399999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="16" t="s">
         <v>66</v>
       </c>
@@ -2767,7 +2817,7 @@
         <v>1.29233648959</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="16" t="s">
         <v>66</v>
       </c>
@@ -2778,7 +2828,7 @@
         <v>1.29233648959</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="12" t="s">
         <v>67</v>
       </c>
@@ -2790,7 +2840,7 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="12" t="s">
         <v>67</v>
       </c>
@@ -2802,7 +2852,7 @@
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="12" t="s">
         <v>67</v>
       </c>
@@ -2814,7 +2864,7 @@
       </c>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="12" t="s">
         <v>67</v>
       </c>
@@ -2826,7 +2876,7 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="12" t="s">
         <v>67</v>
       </c>
@@ -2838,7 +2888,7 @@
       </c>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="12" t="s">
         <v>67</v>
       </c>
@@ -2850,7 +2900,7 @@
       </c>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -2859,7 +2909,7 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -2868,7 +2918,7 @@
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -2877,7 +2927,7 @@
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -2886,7 +2936,7 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -2895,7 +2945,7 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -2904,7 +2954,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
         <v>59</v>
       </c>
@@ -2916,7 +2966,7 @@
       </c>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="9" t="s">
         <v>59</v>
       </c>
@@ -2928,7 +2978,7 @@
       </c>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="9" t="s">
         <v>59</v>
       </c>
@@ -2940,7 +2990,7 @@
       </c>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="9" t="s">
         <v>59</v>
       </c>
@@ -2952,7 +3002,7 @@
       </c>
       <c r="D23" s="9"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="9" t="s">
         <v>59</v>
       </c>
@@ -2964,7 +3014,7 @@
       </c>
       <c r="D24" s="9"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="9" t="s">
         <v>59</v>
       </c>
@@ -3060,13 +3110,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -3078,16 +3128,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3098,7 +3148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -3109,7 +3159,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -3120,7 +3170,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -3142,16 +3192,181 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7939C9-F2CF-5E44-A766-15594E509A3A}">
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3165,7 +3380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3179,7 +3394,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -3193,7 +3408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3207,7 +3422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -3221,7 +3436,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -3235,7 +3450,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -3246,7 +3461,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -3257,7 +3472,7 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -3268,7 +3483,7 @@
         <v>0.35599999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -3289,17 +3504,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3313,7 +3528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -3330,7 +3545,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -3347,7 +3562,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -3361,7 +3576,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -3386,17 +3601,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3407,7 +3622,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -3421,7 +3636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -3432,7 +3647,7 @@
         <v>9.7500000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -3441,59 +3656,6 @@
       </c>
       <c r="C4" s="2">
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2">
-        <v>16.5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3">
-        <v>1.2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3507,19 +3669,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.5" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3530,36 +3689,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16.5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5">
-        <v>5.9</v>
+      <c r="C3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3573,142 +3722,63 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.1789042974999999</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.16683899284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1.75</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.95670999999999995</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.82430000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="10">
-        <v>30</v>
-      </c>
-      <c r="D8" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="10">
-        <v>30</v>
-      </c>
-      <c r="D9" s="10">
-        <v>30</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>5.9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3718,40 +3788,137 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.1789042974999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.16683899284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="s">
-        <v>63</v>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.95670999999999995</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.82430000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="10">
+        <v>30</v>
+      </c>
+      <c r="D8" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="10">
+        <v>30</v>
+      </c>
+      <c r="D9" s="10">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes to the sample-age-comps.R
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3686" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3694" uniqueCount="127">
   <si>
     <t>Par</t>
   </si>
@@ -449,6 +449,12 @@
   </si>
   <si>
     <t>AIBS</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>number</t>
   </si>
 </sst>
 </file>
@@ -3252,15 +3258,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1117"/>
+  <dimension ref="A1:I1117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -3280,7 +3286,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -3299,8 +3305,14 @@
       <c r="F2">
         <v>0.74444063513513603</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3319,8 +3331,14 @@
       <c r="F3">
         <v>0.192327878378379</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -3339,8 +3357,14 @@
       <c r="F4">
         <v>0.502253689189189</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -3359,8 +3383,14 @@
       <c r="F5">
         <v>0.30669139189189198</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -3379,8 +3409,14 @@
       <c r="F6">
         <v>0.66303685135135104</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -3399,8 +3435,14 @@
       <c r="F7">
         <v>0.783576621621622</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -3419,8 +3461,14 @@
       <c r="F8">
         <v>6.9345658108108804E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -3440,7 +3488,7 @@
         <v>0.15883759729729699</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -3460,7 +3508,7 @@
         <v>2.40655175675672E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -3480,7 +3528,7 @@
         <v>1.8061236486488E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -3500,7 +3548,7 @@
         <v>1.5039932432429699E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>85</v>
       </c>
@@ -3520,7 +3568,7 @@
         <v>0.120035</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -3540,7 +3588,7 @@
         <v>0.50449105405405403</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -3560,7 +3608,7 @@
         <v>0.14663374324324299</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
added recruitment data to the data input spreadsheet for the conditioning part of the model
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" firstSheet="7" activeTab="14"/>
+    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,9 @@
     <sheet name="FisherySelexType" sheetId="14" r:id="rId13"/>
     <sheet name="qFishery" sheetId="15" r:id="rId14"/>
     <sheet name="Movement" sheetId="16" r:id="rId15"/>
+    <sheet name="Conditioning_recruitment" sheetId="20" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3694" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3696" uniqueCount="129">
   <si>
     <t>Par</t>
   </si>
@@ -455,6 +456,12 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>Recruitment</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -3260,7 +3267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -25655,6 +25662,365 @@
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1977</v>
+      </c>
+      <c r="B2">
+        <v>4.41974</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1978</v>
+      </c>
+      <c r="B3">
+        <v>5.29922</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1979</v>
+      </c>
+      <c r="B4">
+        <v>86.385999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1980</v>
+      </c>
+      <c r="B5">
+        <v>25.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1981</v>
+      </c>
+      <c r="B6">
+        <v>9.9050999999999991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1982</v>
+      </c>
+      <c r="B7">
+        <v>42.302999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1983</v>
+      </c>
+      <c r="B8">
+        <v>23.972799999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1984</v>
+      </c>
+      <c r="B9">
+        <v>43.513800000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1985</v>
+      </c>
+      <c r="B10">
+        <v>2.3374799999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1986</v>
+      </c>
+      <c r="B11">
+        <v>19.530419999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1987</v>
+      </c>
+      <c r="B12">
+        <v>18.80922</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1988</v>
+      </c>
+      <c r="B13">
+        <v>3.6227999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1989</v>
+      </c>
+      <c r="B14">
+        <v>4.5216200000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1990</v>
+      </c>
+      <c r="B15">
+        <v>6.8762600000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1991</v>
+      </c>
+      <c r="B16">
+        <v>27.2682</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1992</v>
+      </c>
+      <c r="B17">
+        <v>1.286332</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1993</v>
+      </c>
+      <c r="B18">
+        <v>23.789200000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1994</v>
+      </c>
+      <c r="B19">
+        <v>4.5983599999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1995</v>
+      </c>
+      <c r="B20">
+        <v>5.3136400000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1996</v>
+      </c>
+      <c r="B21">
+        <v>7.73184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1997</v>
+      </c>
+      <c r="B22">
+        <v>16.884160000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1998</v>
+      </c>
+      <c r="B23">
+        <v>2.3016200000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1999</v>
+      </c>
+      <c r="B24">
+        <v>29.922999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2000</v>
+      </c>
+      <c r="B25">
+        <v>16.93562</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2001</v>
+      </c>
+      <c r="B26">
+        <v>10.152659999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2002</v>
+      </c>
+      <c r="B27">
+        <v>41.469200000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2003</v>
+      </c>
+      <c r="B28">
+        <v>6.3422200000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2004</v>
+      </c>
+      <c r="B29">
+        <v>12.67834</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2005</v>
+      </c>
+      <c r="B30">
+        <v>6.0571400000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2006</v>
+      </c>
+      <c r="B31">
+        <v>10.717280000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2007</v>
+      </c>
+      <c r="B32">
+        <v>7.7943800000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2008</v>
+      </c>
+      <c r="B33">
+        <v>8.4423200000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2009</v>
+      </c>
+      <c r="B34">
+        <v>7.8210800000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2010</v>
+      </c>
+      <c r="B35">
+        <v>17.842919999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2011</v>
+      </c>
+      <c r="B36">
+        <v>5.0390600000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2012</v>
+      </c>
+      <c r="B37">
+        <v>9.2936599999999991</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2013</v>
+      </c>
+      <c r="B38">
+        <v>1.0178100000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2014</v>
+      </c>
+      <c r="B39">
+        <v>7.9882400000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2015</v>
+      </c>
+      <c r="B40">
+        <v>13.20866</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2016</v>
+      </c>
+      <c r="B41">
+        <v>150.34299999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2017</v>
+      </c>
+      <c r="B42">
+        <v>40.119799999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2018</v>
+      </c>
+      <c r="B43">
+        <v>12.491199999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
working on initial population, but it's not correct yet.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -25675,7 +25675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -26035,7 +26035,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26056,7 +26056,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
still working on initial conditioning. not running yet.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="1"/>
+    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -458,16 +458,16 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Average log-recruitment (either 16.5 or 19.5) - WHAT ARE UNITS??</t>
-  </si>
-  <si>
     <t>Nstart</t>
   </si>
   <si>
     <t>Starting numbers (millions) check units</t>
   </si>
   <si>
-    <t>Starting biomass (kt) check units</t>
+    <t>Starting biomass (kt) check units (which is 396,000,000 kg)</t>
+  </si>
+  <si>
+    <t>Average log-recruitment (either 16.5 or 19.5) - WHAT ARE UNITS?? Million?</t>
   </si>
 </sst>
 </file>
@@ -26034,8 +26034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26070,18 +26070,18 @@
         <v>396</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="2">
         <v>111.157</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -26586,7 +26586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -26611,7 +26611,7 @@
         <v>16.5</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
still trying to get comps sampling right, and to get the .dat file builders right, and the initial population right.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="6"/>
+    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -26034,8 +26034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26586,8 +26586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26619,7 +26619,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
'I really f'ed it up this time, didn't I my dear'
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -25676,7 +25676,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26035,7 +26035,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Have the conditioning portion mostly working, using F. Needs work on the age comps sampling. and movement needs to be added.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -25675,8 +25675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26035,7 +26035,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26608,7 +26608,7 @@
         <v>32</v>
       </c>
       <c r="B2">
-        <v>16.5</v>
+        <v>160.5</v>
       </c>
       <c r="C2" t="s">
         <v>130</v>
@@ -26619,7 +26619,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
UPdated EM data through 2018, finished the age comp sampling code, fixed the dat file builder for the conditioning period, got the forward projection stuff running. Needs to link with and EM and apportionment next.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="1"/>
+    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -26034,8 +26034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26586,8 +26586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26608,7 +26608,7 @@
         <v>32</v>
       </c>
       <c r="B2">
-        <v>160.5</v>
+        <v>16.5</v>
       </c>
       <c r="C2" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
can now call the EM from the sim loop, but still need to tweak the forward projecting section's .dat file maker code.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="6"/>
+    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -26034,8 +26034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26056,7 +26056,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -26089,7 +26089,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -26586,7 +26586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
broke the .dat files into two parts, one that is updated, one that is fixed (unchanging) added the EM to the sim loop.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -26035,7 +26035,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26089,7 +26089,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
fixed scale issue in conditioning period. Index scale still off. Dat file builder isn't working.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3698" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3747" uniqueCount="170">
   <si>
     <t>Par</t>
   </si>
@@ -469,6 +469,123 @@
   <si>
     <t>Average log-recruitment (either 16.5 or 19.5) - WHAT ARE UNITS?? Million?</t>
   </si>
+  <si>
+    <t>apport.opt</t>
+  </si>
+  <si>
+    <t>apportionment option to use for forward simulations</t>
+  </si>
+  <si>
+    <t>apportionment option list</t>
+  </si>
+  <si>
+    <t>equal apport to all areas</t>
+  </si>
+  <si>
+    <t>fixed at the 2013 values</t>
+  </si>
+  <si>
+    <t>equilibrium (stationary movement matrix)</t>
+  </si>
+  <si>
+    <t>NPFMC method</t>
+  </si>
+  <si>
+    <t>survey only, 5 year expon wt</t>
+  </si>
+  <si>
+    <t>fishery only, 5 year expon wt</t>
+  </si>
+  <si>
+    <t>non-expon wt NPFMC</t>
+  </si>
+  <si>
+    <t>partially fixed (BS and AI fixed), NPFMC for others</t>
+  </si>
+  <si>
+    <t>age/length based maturity</t>
+  </si>
+  <si>
+    <t>random effects (not coded in yet)</t>
+  </si>
+  <si>
+    <t>all to one area</t>
+  </si>
+  <si>
+    <t>penalized (not operational)</t>
+  </si>
+  <si>
+    <t>terminal year surv biom proportions (not operational)</t>
+  </si>
+  <si>
+    <t>non-expon wt age/length based (not operational)</t>
+  </si>
+  <si>
+    <t>current.props1</t>
+  </si>
+  <si>
+    <t>current.props2</t>
+  </si>
+  <si>
+    <t>current.props3</t>
+  </si>
+  <si>
+    <t>current.props4</t>
+  </si>
+  <si>
+    <t>current.props5</t>
+  </si>
+  <si>
+    <t>current.props6</t>
+  </si>
+  <si>
+    <t>input value for apportionment option 2 (fixed at 2013 values)</t>
+  </si>
+  <si>
+    <t>equilib.props1</t>
+  </si>
+  <si>
+    <t>equilib.props2</t>
+  </si>
+  <si>
+    <t>equilib.props3</t>
+  </si>
+  <si>
+    <t>equilib.props4</t>
+  </si>
+  <si>
+    <t>equilib.props5</t>
+  </si>
+  <si>
+    <t>equilib.props6</t>
+  </si>
+  <si>
+    <t>input value for apportionment option 3 (movement equilib)</t>
+  </si>
+  <si>
+    <t>FixedA1</t>
+  </si>
+  <si>
+    <t>FixedA2</t>
+  </si>
+  <si>
+    <t>input value for option 8 Area 1 (Bering) fixed proportion for apportionment</t>
+  </si>
+  <si>
+    <t>input value for option 8 Area 2 (Aleutians) fixed proportion for apportionment</t>
+  </si>
+  <si>
+    <t>A_L.mat</t>
+  </si>
+  <si>
+    <t>input value for option 9 - ROW number of the age or length bin for 50% maturity</t>
+  </si>
+  <si>
+    <t>lucky.area</t>
+  </si>
+  <si>
+    <t>input value for option 11 - the lucky area that gets 100% of ABC</t>
+  </si>
 </sst>
 </file>
 
@@ -578,7 +695,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,6 +731,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,7 +851,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -780,6 +903,7 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="40" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -26032,15 +26156,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -26050,19 +26177,28 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -26072,8 +26208,14 @@
       <c r="C3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>127</v>
       </c>
@@ -26083,8 +26225,14 @@
       <c r="C4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -26093,6 +26241,259 @@
       </c>
       <c r="C5" t="s">
         <v>18</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7">
+        <v>0.1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8">
+        <v>0.13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>154</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9">
+        <v>0.11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10">
+        <v>0.34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>154</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11">
+        <v>0.11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12">
+        <v>0.21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>154</v>
+      </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13">
+        <v>9.2315344999999993E-2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>161</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13" s="29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14">
+        <v>0.13670328400000001</v>
+      </c>
+      <c r="C14" t="s">
+        <v>161</v>
+      </c>
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15">
+        <v>0.13052393000000001</v>
+      </c>
+      <c r="C15" t="s">
+        <v>161</v>
+      </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16">
+        <v>0.26827582300000002</v>
+      </c>
+      <c r="C16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B17">
+        <v>0.137707199</v>
+      </c>
+      <c r="C17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18">
+        <v>0.23447441899999999</v>
+      </c>
+      <c r="C18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19">
+        <v>0.1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20">
+        <v>0.1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed the read-in issue with the .dat file builder
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="1"/>
+    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -26158,8 +26158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26186,7 +26186,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -26237,7 +26237,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -26987,8 +26987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -27020,7 +27020,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
OMFG it's running!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!! For multiple years. : )
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="6"/>
+    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -26158,7 +26158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -26186,7 +26186,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -26987,7 +26987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added code for conditioning period figures, added a sablefish input excel file that can be switched on to try to match the management model single area parameter values.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -26159,7 +26159,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26186,7 +26186,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -26237,7 +26237,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
fixed the scale on the indices, though variability is still a bit high.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="1"/>
+    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3747" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3813" uniqueCount="174">
   <si>
     <t>Par</t>
   </si>
@@ -585,6 +585,18 @@
   </si>
   <si>
     <t>input value for option 11 - the lucky area that gets 100% of ABC</t>
+  </si>
+  <si>
+    <t>not log-scale</t>
+  </si>
+  <si>
+    <t>log scale values</t>
+  </si>
+  <si>
+    <t>not on log scale</t>
+  </si>
+  <si>
+    <t>log scale</t>
   </si>
 </sst>
 </file>
@@ -1489,15 +1501,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>63</v>
       </c>
@@ -1510,8 +1522,11 @@
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1519,10 +1534,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
+        <v>8.5848583971778929</v>
+      </c>
+      <c r="D2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="1">
         <v>2.15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -1530,10 +1551,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
+        <v>8.5848583971778929</v>
+      </c>
+      <c r="E3" s="1">
         <v>2.15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -1541,10 +1565,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
+        <v>8.5848583971778929</v>
+      </c>
+      <c r="E4" s="1">
         <v>2.15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -1552,10 +1579,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="1">
+        <v>8.5848583971778929</v>
+      </c>
+      <c r="E5" s="1">
         <v>2.15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
@@ -1563,10 +1593,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="1">
+        <v>8.5848583971778929</v>
+      </c>
+      <c r="E6" s="1">
         <v>2.15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -1574,10 +1607,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="1">
+        <v>8.5848583971778929</v>
+      </c>
+      <c r="E7" s="1">
         <v>2.15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>52</v>
       </c>
@@ -1585,10 +1621,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="18">
+        <v>5.0530903165638676</v>
+      </c>
+      <c r="E8" s="18">
         <v>1.62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>52</v>
       </c>
@@ -1596,10 +1635,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="18">
+        <v>5.0530903165638676</v>
+      </c>
+      <c r="E9" s="18">
         <v>1.62</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>52</v>
       </c>
@@ -1607,10 +1649,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="18">
+        <v>5.0530903165638676</v>
+      </c>
+      <c r="E10" s="18">
         <v>1.62</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>52</v>
       </c>
@@ -1618,10 +1663,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="18">
+        <v>5.0530903165638676</v>
+      </c>
+      <c r="E11" s="18">
         <v>1.62</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>52</v>
       </c>
@@ -1629,10 +1677,13 @@
         <v>5</v>
       </c>
       <c r="C12" s="18">
+        <v>5.0530903165638676</v>
+      </c>
+      <c r="E12" s="18">
         <v>1.62</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>52</v>
       </c>
@@ -1640,6 +1691,9 @@
         <v>6</v>
       </c>
       <c r="C13" s="18">
+        <v>5.0530903165638676</v>
+      </c>
+      <c r="E13" s="18">
         <v>1.62</v>
       </c>
     </row>
@@ -1656,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+      <selection activeCell="D2" sqref="D2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1667,7 +1721,7 @@
     <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>63</v>
       </c>
@@ -1686,8 +1740,11 @@
       <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>64</v>
       </c>
@@ -1698,13 +1755,22 @@
         <v>48</v>
       </c>
       <c r="D2" s="12">
+        <v>2.299476606544725</v>
+      </c>
+      <c r="E2" s="12">
+        <v>9.8205935562528204</v>
+      </c>
+      <c r="F2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H2" s="12">
         <v>0.83268153466700001</v>
       </c>
-      <c r="E2" s="12">
+      <c r="I2" s="12">
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>64</v>
       </c>
@@ -1715,13 +1781,22 @@
         <v>49</v>
       </c>
       <c r="D3" s="13">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1.6718653849036007</v>
+      </c>
+      <c r="F3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H3" s="13">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E3" s="13">
+      <c r="I3" s="13">
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>64</v>
       </c>
@@ -1733,8 +1808,13 @@
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>64</v>
       </c>
@@ -1745,13 +1825,22 @@
         <v>48</v>
       </c>
       <c r="D5" s="12">
+        <v>2.299476606544725</v>
+      </c>
+      <c r="E5" s="12">
+        <v>9.8205935562528204</v>
+      </c>
+      <c r="F5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H5" s="12">
         <v>0.83268153466700001</v>
       </c>
-      <c r="E5" s="12">
+      <c r="I5" s="12">
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>64</v>
       </c>
@@ -1762,13 +1851,22 @@
         <v>49</v>
       </c>
       <c r="D6" s="13">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1.6718653849036007</v>
+      </c>
+      <c r="F6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H6" s="13">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E6" s="13">
+      <c r="I6" s="13">
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>64</v>
       </c>
@@ -1780,8 +1878,13 @@
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>64</v>
       </c>
@@ -1792,13 +1895,22 @@
         <v>48</v>
       </c>
       <c r="D8" s="12">
+        <v>2.299476606544725</v>
+      </c>
+      <c r="E8" s="12">
+        <v>9.8205935562528204</v>
+      </c>
+      <c r="F8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H8" s="12">
         <v>0.83268153466700001</v>
       </c>
-      <c r="E8" s="12">
+      <c r="I8" s="12">
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>64</v>
       </c>
@@ -1809,13 +1921,22 @@
         <v>49</v>
       </c>
       <c r="D9" s="13">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E9" s="13">
+        <v>1.6718653849036007</v>
+      </c>
+      <c r="F9" t="s">
+        <v>170</v>
+      </c>
+      <c r="H9" s="13">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E9" s="13">
+      <c r="I9" s="13">
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>64</v>
       </c>
@@ -1827,8 +1948,13 @@
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>170</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>64</v>
       </c>
@@ -1839,13 +1965,22 @@
         <v>48</v>
       </c>
       <c r="D11" s="12">
+        <v>2.299476606544725</v>
+      </c>
+      <c r="E11" s="12">
+        <v>9.8205935562528204</v>
+      </c>
+      <c r="F11" t="s">
+        <v>170</v>
+      </c>
+      <c r="H11" s="12">
         <v>0.83268153466700001</v>
       </c>
-      <c r="E11" s="12">
+      <c r="I11" s="12">
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>64</v>
       </c>
@@ -1856,13 +1991,22 @@
         <v>49</v>
       </c>
       <c r="D12" s="13">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1.6718653849036007</v>
+      </c>
+      <c r="F12" t="s">
+        <v>170</v>
+      </c>
+      <c r="H12" s="13">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E12" s="13">
+      <c r="I12" s="13">
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>64</v>
       </c>
@@ -1874,8 +2018,13 @@
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>170</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>64</v>
       </c>
@@ -1886,13 +2035,22 @@
         <v>48</v>
       </c>
       <c r="D14" s="12">
+        <v>2.299476606544725</v>
+      </c>
+      <c r="E14" s="12">
+        <v>9.8205935562528204</v>
+      </c>
+      <c r="F14" t="s">
+        <v>170</v>
+      </c>
+      <c r="H14" s="12">
         <v>0.83268153466700001</v>
       </c>
-      <c r="E14" s="12">
+      <c r="I14" s="12">
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>64</v>
       </c>
@@ -1903,13 +2061,22 @@
         <v>49</v>
       </c>
       <c r="D15" s="13">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E15" s="13">
+        <v>1.6718653849036007</v>
+      </c>
+      <c r="F15" t="s">
+        <v>170</v>
+      </c>
+      <c r="H15" s="13">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E15" s="13">
+      <c r="I15" s="13">
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>64</v>
       </c>
@@ -1921,8 +2088,13 @@
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>170</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>64</v>
       </c>
@@ -1933,13 +2105,22 @@
         <v>48</v>
       </c>
       <c r="D17" s="12">
+        <v>2.299476606544725</v>
+      </c>
+      <c r="E17" s="12">
+        <v>9.8205935562528204</v>
+      </c>
+      <c r="F17" t="s">
+        <v>170</v>
+      </c>
+      <c r="H17" s="12">
         <v>0.83268153466700001</v>
       </c>
-      <c r="E17" s="12">
+      <c r="I17" s="12">
         <v>2.28448156415</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>64</v>
       </c>
@@ -1950,13 +2131,22 @@
         <v>49</v>
       </c>
       <c r="D18" s="13">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E18" s="13">
+        <v>1.6718653849036007</v>
+      </c>
+      <c r="F18" t="s">
+        <v>170</v>
+      </c>
+      <c r="H18" s="13">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E18" s="13">
+      <c r="I18" s="13">
         <v>0.51393999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>64</v>
       </c>
@@ -1968,8 +2158,13 @@
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>170</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>65</v>
       </c>
@@ -1980,13 +2175,22 @@
         <v>48</v>
       </c>
       <c r="D20" s="20">
+        <v>2.3470833330266236</v>
+      </c>
+      <c r="E20" s="20">
+        <v>2.2986856730216711</v>
+      </c>
+      <c r="F20" t="s">
+        <v>170</v>
+      </c>
+      <c r="H20" s="20">
         <v>0.85317342242799998</v>
       </c>
-      <c r="E20" s="20">
+      <c r="I20" s="20">
         <v>0.83233751308500004</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>65</v>
       </c>
@@ -1997,13 +2201,22 @@
         <v>49</v>
       </c>
       <c r="D21" s="20">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E21" s="20">
+        <v>3.1478153783457579</v>
+      </c>
+      <c r="F21" t="s">
+        <v>170</v>
+      </c>
+      <c r="H21" s="20">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E21" s="20">
+      <c r="I21" s="20">
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>65</v>
       </c>
@@ -2015,8 +2228,13 @@
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>170</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>65</v>
       </c>
@@ -2027,13 +2245,22 @@
         <v>48</v>
       </c>
       <c r="D23" s="22">
+        <v>2.3470833330266236</v>
+      </c>
+      <c r="E23" s="22">
+        <v>2.2986856730216711</v>
+      </c>
+      <c r="F23" t="s">
+        <v>170</v>
+      </c>
+      <c r="H23" s="22">
         <v>0.85317342242799998</v>
       </c>
-      <c r="E23" s="22">
+      <c r="I23" s="22">
         <v>0.83233751308500004</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>65</v>
       </c>
@@ -2044,13 +2271,22 @@
         <v>49</v>
       </c>
       <c r="D24" s="23">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E24" s="23">
+        <v>3.1478153783457579</v>
+      </c>
+      <c r="F24" t="s">
+        <v>170</v>
+      </c>
+      <c r="H24" s="23">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E24" s="23">
+      <c r="I24" s="23">
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>65</v>
       </c>
@@ -2062,8 +2298,13 @@
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>170</v>
+      </c>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>65</v>
       </c>
@@ -2073,14 +2314,23 @@
       <c r="C26" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="22">
+        <v>2.3470833330266236</v>
+      </c>
+      <c r="E26" s="22">
+        <v>2.2986856730216711</v>
+      </c>
+      <c r="F26" t="s">
+        <v>170</v>
+      </c>
+      <c r="H26" s="25">
         <v>0.85317342242799998</v>
       </c>
-      <c r="E26" s="25">
+      <c r="I26" s="25">
         <v>0.83233751308500004</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>65</v>
       </c>
@@ -2090,14 +2340,23 @@
       <c r="C27" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="23">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E27" s="23">
+        <v>3.1478153783457579</v>
+      </c>
+      <c r="F27" t="s">
+        <v>170</v>
+      </c>
+      <c r="H27" s="26">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E27" s="25">
+      <c r="I27" s="25">
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>65</v>
       </c>
@@ -2109,8 +2368,13 @@
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>170</v>
+      </c>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>65</v>
       </c>
@@ -2120,14 +2384,23 @@
       <c r="C29" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="22">
+        <v>2.3470833330266236</v>
+      </c>
+      <c r="E29" s="22">
+        <v>2.2986856730216711</v>
+      </c>
+      <c r="F29" t="s">
+        <v>170</v>
+      </c>
+      <c r="H29" s="27">
         <v>1.1324375825599999</v>
       </c>
-      <c r="E29" s="27">
+      <c r="I29" s="27">
         <v>1.1762722908800001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>65</v>
       </c>
@@ -2137,14 +2410,23 @@
       <c r="C30" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="23">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E30" s="23">
+        <v>3.1478153783457579</v>
+      </c>
+      <c r="F30" t="s">
+        <v>170</v>
+      </c>
+      <c r="H30" s="26">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E30" s="25">
+      <c r="I30" s="25">
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>65</v>
       </c>
@@ -2156,8 +2438,13 @@
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>170</v>
+      </c>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>65</v>
       </c>
@@ -2167,14 +2454,23 @@
       <c r="C32" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="22">
+        <v>2.3470833330266236</v>
+      </c>
+      <c r="E32" s="22">
+        <v>2.2986856730216711</v>
+      </c>
+      <c r="F32" t="s">
+        <v>170</v>
+      </c>
+      <c r="H32" s="25">
         <v>1.4339075566299999</v>
       </c>
-      <c r="E32" s="27">
+      <c r="I32" s="27">
         <v>1.29701630606</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>65</v>
       </c>
@@ -2184,14 +2480,23 @@
       <c r="C33" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="26">
+      <c r="D33" s="23">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E33" s="23">
+        <v>3.1478153783457579</v>
+      </c>
+      <c r="F33" t="s">
+        <v>170</v>
+      </c>
+      <c r="H33" s="26">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E33" s="25">
+      <c r="I33" s="25">
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>65</v>
       </c>
@@ -2203,8 +2508,13 @@
       </c>
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>170</v>
+      </c>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>65</v>
       </c>
@@ -2214,14 +2524,23 @@
       <c r="C35" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="22">
+        <v>2.3470833330266236</v>
+      </c>
+      <c r="E35" s="22">
+        <v>2.2986856730216711</v>
+      </c>
+      <c r="F35" t="s">
+        <v>170</v>
+      </c>
+      <c r="H35" s="25">
         <v>1.4339075566299999</v>
       </c>
-      <c r="E35" s="27">
+      <c r="I35" s="27">
         <v>1.29701630606</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>65</v>
       </c>
@@ -2231,14 +2550,23 @@
       <c r="C36" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="26">
+      <c r="D36" s="23">
+        <v>2.4209983586692707</v>
+      </c>
+      <c r="E36" s="23">
+        <v>3.1478153783457579</v>
+      </c>
+      <c r="F36" t="s">
+        <v>170</v>
+      </c>
+      <c r="H36" s="26">
         <v>0.88417999999999997</v>
       </c>
-      <c r="E36" s="25">
+      <c r="I36" s="25">
         <v>1.1467086815500001</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>65</v>
       </c>
@@ -2250,8 +2578,13 @@
       </c>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>170</v>
+      </c>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>55</v>
       </c>
@@ -2266,8 +2599,10 @@
       <c r="F38" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>55</v>
       </c>
@@ -2278,16 +2613,22 @@
         <v>49</v>
       </c>
       <c r="D39" s="12">
+        <v>4.0836779135333341</v>
+      </c>
+      <c r="E39" s="12">
+        <v>3.8168785874624138</v>
+      </c>
+      <c r="F39" t="s">
+        <v>170</v>
+      </c>
+      <c r="H39" s="12">
         <v>1.4069980317499999</v>
       </c>
-      <c r="E39" s="12">
+      <c r="I39" s="12">
         <v>1.3394329648900001</v>
       </c>
-      <c r="F39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>55</v>
       </c>
@@ -2298,16 +2639,22 @@
         <v>50</v>
       </c>
       <c r="D40" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="E40" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="F40" t="s">
+        <v>170</v>
+      </c>
+      <c r="H40" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="E40" s="12">
+      <c r="I40" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="F40" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>55</v>
       </c>
@@ -2320,10 +2667,12 @@
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>55</v>
       </c>
@@ -2334,16 +2683,22 @@
         <v>49</v>
       </c>
       <c r="D42" s="12">
+        <v>4.0836779135333341</v>
+      </c>
+      <c r="E42" s="12">
+        <v>3.8168785874624138</v>
+      </c>
+      <c r="F42" t="s">
+        <v>170</v>
+      </c>
+      <c r="H42" s="12">
         <v>1.4069980317499999</v>
       </c>
-      <c r="E42" s="12">
+      <c r="I42" s="12">
         <v>1.3394329648900001</v>
       </c>
-      <c r="F42" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>55</v>
       </c>
@@ -2354,16 +2709,22 @@
         <v>50</v>
       </c>
       <c r="D43" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="E43" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="F43" t="s">
+        <v>170</v>
+      </c>
+      <c r="H43" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="E43" s="12">
+      <c r="I43" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="F43" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>55</v>
       </c>
@@ -2376,10 +2737,12 @@
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="F44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>55</v>
       </c>
@@ -2390,16 +2753,22 @@
         <v>49</v>
       </c>
       <c r="D45" s="12">
+        <v>4.0836779135333341</v>
+      </c>
+      <c r="E45" s="12">
+        <v>3.8168785874624138</v>
+      </c>
+      <c r="F45" t="s">
+        <v>170</v>
+      </c>
+      <c r="H45" s="12">
         <v>1.4069980317499999</v>
       </c>
-      <c r="E45" s="12">
+      <c r="I45" s="12">
         <v>1.3394329648900001</v>
       </c>
-      <c r="F45" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>55</v>
       </c>
@@ -2410,16 +2779,22 @@
         <v>50</v>
       </c>
       <c r="D46" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="E46" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="F46" t="s">
+        <v>170</v>
+      </c>
+      <c r="H46" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="E46" s="12">
+      <c r="I46" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="F46" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>55</v>
       </c>
@@ -2432,10 +2807,12 @@
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>55</v>
       </c>
@@ -2446,16 +2823,22 @@
         <v>49</v>
       </c>
       <c r="D48" s="12">
+        <v>4.0836779135333341</v>
+      </c>
+      <c r="E48" s="12">
+        <v>3.8168785874624138</v>
+      </c>
+      <c r="F48" t="s">
+        <v>170</v>
+      </c>
+      <c r="H48" s="12">
         <v>1.4069980317499999</v>
       </c>
-      <c r="E48" s="12">
+      <c r="I48" s="12">
         <v>1.3394329648900001</v>
       </c>
-      <c r="F48" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>55</v>
       </c>
@@ -2466,16 +2849,22 @@
         <v>50</v>
       </c>
       <c r="D49" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="E49" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="F49" t="s">
+        <v>170</v>
+      </c>
+      <c r="H49" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="E49" s="12">
+      <c r="I49" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="F49" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>55</v>
       </c>
@@ -2488,10 +2877,12 @@
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>55</v>
       </c>
@@ -2502,16 +2893,22 @@
         <v>49</v>
       </c>
       <c r="D51" s="12">
+        <v>4.0836779135333341</v>
+      </c>
+      <c r="E51" s="12">
+        <v>3.8168785874624138</v>
+      </c>
+      <c r="F51" t="s">
+        <v>170</v>
+      </c>
+      <c r="H51" s="12">
         <v>1.4069980317499999</v>
       </c>
-      <c r="E51" s="12">
+      <c r="I51" s="12">
         <v>1.3394329648900001</v>
       </c>
-      <c r="F51" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>55</v>
       </c>
@@ -2522,16 +2919,22 @@
         <v>50</v>
       </c>
       <c r="D52" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="E52" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="F52" t="s">
+        <v>170</v>
+      </c>
+      <c r="H52" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="E52" s="12">
+      <c r="I52" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="F52" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>55</v>
       </c>
@@ -2544,10 +2947,12 @@
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>55</v>
       </c>
@@ -2558,16 +2963,22 @@
         <v>49</v>
       </c>
       <c r="D54" s="12">
+        <v>4.0836779135333341</v>
+      </c>
+      <c r="E54" s="12">
+        <v>3.8168785874624138</v>
+      </c>
+      <c r="F54" t="s">
+        <v>170</v>
+      </c>
+      <c r="H54" s="12">
         <v>1.4069980317499999</v>
       </c>
-      <c r="E54" s="12">
+      <c r="I54" s="12">
         <v>1.3394329648900001</v>
       </c>
-      <c r="F54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>55</v>
       </c>
@@ -2578,16 +2989,22 @@
         <v>50</v>
       </c>
       <c r="D55" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="E55" s="12">
+        <v>5.7072584870432808</v>
+      </c>
+      <c r="F55" t="s">
+        <v>170</v>
+      </c>
+      <c r="H55" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="E55" s="12">
+      <c r="I55" s="12">
         <v>1.74173878351</v>
       </c>
-      <c r="F55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>57</v>
       </c>
@@ -2598,13 +3015,22 @@
         <v>48</v>
       </c>
       <c r="D56" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="E56" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="F56" t="s">
+        <v>170</v>
+      </c>
+      <c r="H56" s="14">
         <v>2.1</v>
       </c>
-      <c r="E56" s="14">
+      <c r="I56" s="14">
         <v>2.1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>57</v>
       </c>
@@ -2615,13 +3041,22 @@
         <v>49</v>
       </c>
       <c r="D57" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="E57" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="F57" t="s">
+        <v>170</v>
+      </c>
+      <c r="H57" s="14">
         <v>0.78649999999999998</v>
       </c>
-      <c r="E57" s="14">
+      <c r="I57" s="14">
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>57</v>
       </c>
@@ -2633,8 +3068,13 @@
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>170</v>
+      </c>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>57</v>
       </c>
@@ -2645,13 +3085,22 @@
         <v>48</v>
       </c>
       <c r="D59" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="E59" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="F59" t="s">
+        <v>170</v>
+      </c>
+      <c r="H59" s="14">
         <v>2.1</v>
       </c>
-      <c r="E59" s="14">
+      <c r="I59" s="14">
         <v>2.1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>57</v>
       </c>
@@ -2662,13 +3111,22 @@
         <v>49</v>
       </c>
       <c r="D60" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="E60" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="F60" t="s">
+        <v>170</v>
+      </c>
+      <c r="H60" s="14">
         <v>0.78649999999999998</v>
       </c>
-      <c r="E60" s="14">
+      <c r="I60" s="14">
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>57</v>
       </c>
@@ -2680,8 +3138,13 @@
       </c>
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>170</v>
+      </c>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>57</v>
       </c>
@@ -2692,13 +3155,22 @@
         <v>48</v>
       </c>
       <c r="D62" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="E62" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="F62" t="s">
+        <v>170</v>
+      </c>
+      <c r="H62" s="14">
         <v>2.1</v>
       </c>
-      <c r="E62" s="14">
+      <c r="I62" s="14">
         <v>2.1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>57</v>
       </c>
@@ -2709,13 +3181,22 @@
         <v>49</v>
       </c>
       <c r="D63" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="E63" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="F63" t="s">
+        <v>170</v>
+      </c>
+      <c r="H63" s="14">
         <v>0.78649999999999998</v>
       </c>
-      <c r="E63" s="14">
+      <c r="I63" s="14">
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>57</v>
       </c>
@@ -2727,8 +3208,13 @@
       </c>
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>170</v>
+      </c>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>57</v>
       </c>
@@ -2739,13 +3225,22 @@
         <v>48</v>
       </c>
       <c r="D65" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="E65" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="F65" t="s">
+        <v>170</v>
+      </c>
+      <c r="H65" s="14">
         <v>2.1</v>
       </c>
-      <c r="E65" s="14">
+      <c r="I65" s="14">
         <v>2.1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>57</v>
       </c>
@@ -2756,13 +3251,22 @@
         <v>49</v>
       </c>
       <c r="D66" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="E66" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="F66" t="s">
+        <v>170</v>
+      </c>
+      <c r="H66" s="14">
         <v>0.78649999999999998</v>
       </c>
-      <c r="E66" s="14">
+      <c r="I66" s="14">
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>57</v>
       </c>
@@ -2774,8 +3278,13 @@
       </c>
       <c r="D67" s="15"/>
       <c r="E67" s="15"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>170</v>
+      </c>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>57</v>
       </c>
@@ -2786,13 +3295,22 @@
         <v>48</v>
       </c>
       <c r="D68" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="E68" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="F68" t="s">
+        <v>170</v>
+      </c>
+      <c r="H68" s="14">
         <v>2.1</v>
       </c>
-      <c r="E68" s="14">
+      <c r="I68" s="14">
         <v>2.1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>57</v>
       </c>
@@ -2803,13 +3321,22 @@
         <v>49</v>
       </c>
       <c r="D69" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="E69" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="F69" t="s">
+        <v>170</v>
+      </c>
+      <c r="H69" s="14">
         <v>0.78649999999999998</v>
       </c>
-      <c r="E69" s="14">
+      <c r="I69" s="14">
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>57</v>
       </c>
@@ -2821,8 +3348,13 @@
       </c>
       <c r="D70" s="15"/>
       <c r="E70" s="15"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>170</v>
+      </c>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>57</v>
       </c>
@@ -2833,13 +3365,22 @@
         <v>48</v>
       </c>
       <c r="D71" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="E71" s="14">
+        <v>8.1661699125676517</v>
+      </c>
+      <c r="F71" t="s">
+        <v>170</v>
+      </c>
+      <c r="H71" s="14">
         <v>2.1</v>
       </c>
-      <c r="E71" s="14">
+      <c r="I71" s="14">
         <v>2.1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>57</v>
       </c>
@@ -2850,13 +3391,22 @@
         <v>49</v>
       </c>
       <c r="D72" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="E72" s="14">
+        <v>2.1956980188358153</v>
+      </c>
+      <c r="F72" t="s">
+        <v>170</v>
+      </c>
+      <c r="H72" s="14">
         <v>0.78649999999999998</v>
       </c>
-      <c r="E72" s="14">
+      <c r="I72" s="14">
         <v>0.78649999999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>57</v>
       </c>
@@ -2868,6 +3418,11 @@
       </c>
       <c r="D73" s="15"/>
       <c r="E73" s="15"/>
+      <c r="F73" t="s">
+        <v>170</v>
+      </c>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B37">
@@ -3017,10 +3572,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3028,7 +3583,7 @@
     <col min="1" max="1" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>63</v>
       </c>
@@ -3041,8 +3596,11 @@
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>64</v>
       </c>
@@ -3050,11 +3608,20 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
+        <v>5.5123462978056237</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="1">
         <v>1.7069903579000001</v>
       </c>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>EXP(E2)</f>
+        <v>5.5123462978056237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>64</v>
       </c>
@@ -3062,11 +3629,18 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
+        <v>5.5123462978056237</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="1">
         <v>1.7069903579000001</v>
       </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F25" si="0">EXP(E3)</f>
+        <v>5.5123462978056237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>64</v>
       </c>
@@ -3074,11 +3648,18 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
+        <v>5.5123462978056237</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="1">
         <v>1.7069903579000001</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>5.5123462978056237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>64</v>
       </c>
@@ -3086,10 +3667,17 @@
         <v>4</v>
       </c>
       <c r="C5">
+        <v>3.2714359581103722</v>
+      </c>
+      <c r="E5">
         <v>1.1852290194399999</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>3.2714359581103722</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>64</v>
       </c>
@@ -3097,10 +3685,17 @@
         <v>5</v>
       </c>
       <c r="C6">
+        <v>3.641284447474828</v>
+      </c>
+      <c r="E6">
         <v>1.29233648959</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>3.641284447474828</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>64</v>
       </c>
@@ -3108,10 +3703,17 @@
         <v>6</v>
       </c>
       <c r="C7">
+        <v>3.641284447474828</v>
+      </c>
+      <c r="E7">
         <v>1.29233648959</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>3.641284447474828</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>65</v>
       </c>
@@ -3119,11 +3721,18 @@
         <v>1</v>
       </c>
       <c r="C8" s="7">
+        <v>5.4884647744522335</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="7">
         <v>1.7026485760600001</v>
       </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>5.4884647744522335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>65</v>
       </c>
@@ -3131,11 +3740,18 @@
         <v>2</v>
       </c>
       <c r="C9" s="7">
+        <v>5.4884647744522335</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="7">
         <v>1.7026485760600001</v>
       </c>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>5.4884647744522335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>65</v>
       </c>
@@ -3143,11 +3759,18 @@
         <v>3</v>
       </c>
       <c r="C10" s="7">
+        <v>5.4884647744522335</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="7">
         <v>1.7026485760600001</v>
       </c>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>5.4884647744522335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>65</v>
       </c>
@@ -3155,11 +3778,18 @@
         <v>4</v>
       </c>
       <c r="C11" s="7">
+        <v>5.0622657988146411</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="7">
         <v>1.6218141693999999</v>
       </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>5.0622657988146411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>65</v>
       </c>
@@ -3167,11 +3797,18 @@
         <v>5</v>
       </c>
       <c r="C12" s="7">
+        <v>7.7262469746224802</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="7">
         <v>2.04462323042</v>
       </c>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>7.7262469746224802</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>65</v>
       </c>
@@ -3179,11 +3816,18 @@
         <v>6</v>
       </c>
       <c r="C13" s="7">
+        <v>7.7262469746224802</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="7">
         <v>2.04462323042</v>
       </c>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>7.7262469746224802</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -3192,7 +3836,7 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -3201,7 +3845,7 @@
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -3210,7 +3854,7 @@
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -3219,7 +3863,7 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -3228,7 +3872,7 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -3237,7 +3881,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>57</v>
       </c>
@@ -3245,11 +3889,18 @@
         <v>1</v>
       </c>
       <c r="C20" s="7">
+        <v>13.588276021033481</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="7">
         <v>2.6092073636799999</v>
       </c>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>13.588276021033481</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>57</v>
       </c>
@@ -3257,11 +3908,18 @@
         <v>2</v>
       </c>
       <c r="C21" s="7">
+        <v>13.588276021033481</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="7">
         <v>2.6092073636799999</v>
       </c>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>13.588276021033481</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>57</v>
       </c>
@@ -3269,11 +3927,18 @@
         <v>3</v>
       </c>
       <c r="C22" s="7">
+        <v>13.588276021033481</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="7">
         <v>2.6092073636799999</v>
       </c>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>13.588276021033481</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>57</v>
       </c>
@@ -3281,11 +3946,18 @@
         <v>4</v>
       </c>
       <c r="C23" s="7">
+        <v>13.588276021033481</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="7">
         <v>2.6092073636799999</v>
       </c>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>13.588276021033481</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>57</v>
       </c>
@@ -3293,11 +3965,18 @@
         <v>5</v>
       </c>
       <c r="C24" s="7">
+        <v>13.588276021033481</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="7">
         <v>2.6092073636799999</v>
       </c>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>13.588276021033481</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>57</v>
       </c>
@@ -3305,9 +3984,16 @@
         <v>6</v>
       </c>
       <c r="C25" s="7">
+        <v>13.588276021033481</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="7">
         <v>2.6092073636799999</v>
       </c>
-      <c r="D25" s="9"/>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>13.588276021033481</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
@@ -26158,7 +26844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -27104,10 +27790,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -27115,7 +27801,7 @@
     <col min="1" max="1" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>63</v>
       </c>
@@ -27131,8 +27817,11 @@
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -27140,13 +27829,22 @@
         <v>48</v>
       </c>
       <c r="C2" s="1">
+        <v>3.250810329768528</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3.2118239768019823</v>
+      </c>
+      <c r="E2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" s="1">
         <v>1.1789042974999999</v>
       </c>
-      <c r="D2" s="1">
+      <c r="J2" s="1">
         <v>1.16683899284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -27154,13 +27852,22 @@
         <v>49</v>
       </c>
       <c r="C3" s="1">
+        <v>5.7546026760057307</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.7114701825907419</v>
+      </c>
+      <c r="E3" t="s">
+        <v>170</v>
+      </c>
+      <c r="I3" s="1">
         <v>1.75</v>
       </c>
-      <c r="D3" s="1">
+      <c r="J3" s="1">
         <v>1.55</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -27169,8 +27876,13 @@
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>170</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -27178,13 +27890,22 @@
         <v>48</v>
       </c>
       <c r="C5" s="1">
+        <v>2.6031181111692159</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7.3890560989306504</v>
+      </c>
+      <c r="E5" t="s">
+        <v>170</v>
+      </c>
+      <c r="I5" s="1">
         <v>0.95670999999999995</v>
       </c>
-      <c r="D5" s="1">
+      <c r="J5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -27192,13 +27913,22 @@
         <v>49</v>
       </c>
       <c r="C6" s="1">
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2.2802840077239361</v>
+      </c>
+      <c r="E6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="1">
+      <c r="J6" s="1">
         <v>0.82430000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -27207,8 +27937,13 @@
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>170</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
@@ -27221,8 +27956,14 @@
       <c r="D8" s="10">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I8" s="10">
+        <v>30</v>
+      </c>
+      <c r="J8" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -27233,6 +27974,12 @@
         <v>30</v>
       </c>
       <c r="D9" s="10">
+        <v>30</v>
+      </c>
+      <c r="I9" s="10">
+        <v>30</v>
+      </c>
+      <c r="J9" s="10">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pushing a checkpoint. it's running for multiple sims and years now.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -3574,7 +3574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C25"/>
     </sheetView>
   </sheetViews>
@@ -26844,8 +26844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26872,7 +26872,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -26940,7 +26940,7 @@
         <v>131</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>132</v>

</xml_diff>

<commit_message>
fixed so all the apportionment options run. starting changes to .rep files for accumulating things we want to track.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -584,9 +584,6 @@
     <t>lucky.area</t>
   </si>
   <si>
-    <t>input value for option 11 - the lucky area that gets 100% of ABC</t>
-  </si>
-  <si>
     <t>not log-scale</t>
   </si>
   <si>
@@ -597,6 +594,9 @@
   </si>
   <si>
     <t>log scale</t>
+  </si>
+  <si>
+    <t>input value for option 11 - the lucky area that gets 100% of ABC (in order 1:6 BS AI WG CG WY EY/SEO)</t>
   </si>
 </sst>
 </file>
@@ -1523,7 +1523,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1537,7 +1537,7 @@
         <v>8.5848583971778929</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" s="1">
         <v>2.15</v>
@@ -1741,7 +1741,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1761,7 +1761,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H2" s="12">
         <v>0.83268153466700001</v>
@@ -1787,7 +1787,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H3" s="13">
         <v>0.88417999999999997</v>
@@ -1809,7 +1809,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -1831,7 +1831,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H5" s="12">
         <v>0.83268153466700001</v>
@@ -1857,7 +1857,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H6" s="13">
         <v>0.88417999999999997</v>
@@ -1879,7 +1879,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -1901,7 +1901,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H8" s="12">
         <v>0.83268153466700001</v>
@@ -1927,7 +1927,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H9" s="13">
         <v>0.88417999999999997</v>
@@ -1949,7 +1949,7 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -1971,7 +1971,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H11" s="12">
         <v>0.83268153466700001</v>
@@ -1997,7 +1997,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H12" s="13">
         <v>0.88417999999999997</v>
@@ -2019,7 +2019,7 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -2041,7 +2041,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H14" s="12">
         <v>0.83268153466700001</v>
@@ -2067,7 +2067,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H15" s="13">
         <v>0.88417999999999997</v>
@@ -2089,7 +2089,7 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -2111,7 +2111,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H17" s="12">
         <v>0.83268153466700001</v>
@@ -2137,7 +2137,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H18" s="13">
         <v>0.88417999999999997</v>
@@ -2159,7 +2159,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -2181,7 +2181,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H20" s="20">
         <v>0.85317342242799998</v>
@@ -2207,7 +2207,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H21" s="20">
         <v>0.88417999999999997</v>
@@ -2229,7 +2229,7 @@
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
       <c r="F22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
@@ -2251,7 +2251,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H23" s="22">
         <v>0.85317342242799998</v>
@@ -2277,7 +2277,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H24" s="23">
         <v>0.88417999999999997</v>
@@ -2299,7 +2299,7 @@
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
       <c r="F25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
@@ -2321,7 +2321,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H26" s="25">
         <v>0.85317342242799998</v>
@@ -2347,7 +2347,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H27" s="26">
         <v>0.88417999999999997</v>
@@ -2369,7 +2369,7 @@
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
       <c r="F28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H28" s="27"/>
       <c r="I28" s="27"/>
@@ -2391,7 +2391,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H29" s="27">
         <v>1.1324375825599999</v>
@@ -2417,7 +2417,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H30" s="26">
         <v>0.88417999999999997</v>
@@ -2439,7 +2439,7 @@
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
       <c r="F31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
@@ -2461,7 +2461,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H32" s="25">
         <v>1.4339075566299999</v>
@@ -2487,7 +2487,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H33" s="26">
         <v>0.88417999999999997</v>
@@ -2509,7 +2509,7 @@
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
       <c r="F34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H34" s="27"/>
       <c r="I34" s="27"/>
@@ -2531,7 +2531,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H35" s="25">
         <v>1.4339075566299999</v>
@@ -2557,7 +2557,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H36" s="26">
         <v>0.88417999999999997</v>
@@ -2579,7 +2579,7 @@
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
       <c r="F37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
@@ -2619,7 +2619,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H39" s="12">
         <v>1.4069980317499999</v>
@@ -2645,7 +2645,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H40" s="12">
         <v>1.74173878351</v>
@@ -2667,7 +2667,7 @@
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -2689,7 +2689,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H42" s="12">
         <v>1.4069980317499999</v>
@@ -2715,7 +2715,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H43" s="12">
         <v>1.74173878351</v>
@@ -2737,7 +2737,7 @@
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="F44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
@@ -2759,7 +2759,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H45" s="12">
         <v>1.4069980317499999</v>
@@ -2785,7 +2785,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H46" s="12">
         <v>1.74173878351</v>
@@ -2807,7 +2807,7 @@
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="9"/>
@@ -2829,7 +2829,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H48" s="12">
         <v>1.4069980317499999</v>
@@ -2855,7 +2855,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H49" s="12">
         <v>1.74173878351</v>
@@ -2877,7 +2877,7 @@
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
@@ -2899,7 +2899,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H51" s="12">
         <v>1.4069980317499999</v>
@@ -2925,7 +2925,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F52" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H52" s="12">
         <v>1.74173878351</v>
@@ -2947,7 +2947,7 @@
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
@@ -2969,7 +2969,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H54" s="12">
         <v>1.4069980317499999</v>
@@ -2995,7 +2995,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H55" s="12">
         <v>1.74173878351</v>
@@ -3021,7 +3021,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F56" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H56" s="14">
         <v>2.1</v>
@@ -3047,7 +3047,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F57" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H57" s="14">
         <v>0.78649999999999998</v>
@@ -3069,7 +3069,7 @@
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
       <c r="F58" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
@@ -3091,7 +3091,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F59" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H59" s="14">
         <v>2.1</v>
@@ -3117,7 +3117,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F60" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H60" s="14">
         <v>0.78649999999999998</v>
@@ -3139,7 +3139,7 @@
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
       <c r="F61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
@@ -3161,7 +3161,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H62" s="14">
         <v>2.1</v>
@@ -3187,7 +3187,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F63" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H63" s="14">
         <v>0.78649999999999998</v>
@@ -3209,7 +3209,7 @@
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
       <c r="F64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H64" s="15"/>
       <c r="I64" s="15"/>
@@ -3231,7 +3231,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H65" s="14">
         <v>2.1</v>
@@ -3257,7 +3257,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H66" s="14">
         <v>0.78649999999999998</v>
@@ -3279,7 +3279,7 @@
       <c r="D67" s="15"/>
       <c r="E67" s="15"/>
       <c r="F67" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="15"/>
@@ -3301,7 +3301,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F68" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H68" s="14">
         <v>2.1</v>
@@ -3327,7 +3327,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F69" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H69" s="14">
         <v>0.78649999999999998</v>
@@ -3349,7 +3349,7 @@
       <c r="D70" s="15"/>
       <c r="E70" s="15"/>
       <c r="F70" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H70" s="15"/>
       <c r="I70" s="15"/>
@@ -3371,7 +3371,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F71" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H71" s="14">
         <v>2.1</v>
@@ -3397,7 +3397,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F72" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H72" s="14">
         <v>0.78649999999999998</v>
@@ -3419,7 +3419,7 @@
       <c r="D73" s="15"/>
       <c r="E73" s="15"/>
       <c r="F73" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H73" s="15"/>
       <c r="I73" s="15"/>
@@ -3597,7 +3597,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3611,7 +3611,7 @@
         <v>5.5123462978056237</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" s="1">
         <v>1.7069903579000001</v>
@@ -26940,7 +26940,7 @@
         <v>131</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>132</v>
@@ -27179,7 +27179,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -27818,7 +27818,7 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -27835,7 +27835,7 @@
         <v>3.2118239768019823</v>
       </c>
       <c r="E2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I2" s="1">
         <v>1.1789042974999999</v>
@@ -27858,7 +27858,7 @@
         <v>4.7114701825907419</v>
       </c>
       <c r="E3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I3" s="1">
         <v>1.75</v>
@@ -27877,7 +27877,7 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -27896,7 +27896,7 @@
         <v>7.3890560989306504</v>
       </c>
       <c r="E5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I5" s="1">
         <v>0.95670999999999995</v>
@@ -27919,7 +27919,7 @@
         <v>2.2802840077239361</v>
       </c>
       <c r="E6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
@@ -27938,7 +27938,7 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>

</xml_diff>

<commit_message>
adding perf metrics and figures, phase 1
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -26845,7 +26845,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26872,7 +26872,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -26923,7 +26923,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
updated with more years and sims, and with new figure code
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -26845,7 +26845,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26872,7 +26872,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -26923,7 +26923,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -26940,7 +26940,7 @@
         <v>131</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>132</v>

</xml_diff>

<commit_message>
stopping for the day. still working on coding in perf.metrics.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3813" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3798" uniqueCount="159">
   <si>
     <t>Par</t>
   </si>
@@ -476,51 +476,6 @@
     <t>apportionment option to use for forward simulations</t>
   </si>
   <si>
-    <t>apportionment option list</t>
-  </si>
-  <si>
-    <t>equal apport to all areas</t>
-  </si>
-  <si>
-    <t>fixed at the 2013 values</t>
-  </si>
-  <si>
-    <t>equilibrium (stationary movement matrix)</t>
-  </si>
-  <si>
-    <t>NPFMC method</t>
-  </si>
-  <si>
-    <t>survey only, 5 year expon wt</t>
-  </si>
-  <si>
-    <t>fishery only, 5 year expon wt</t>
-  </si>
-  <si>
-    <t>non-expon wt NPFMC</t>
-  </si>
-  <si>
-    <t>partially fixed (BS and AI fixed), NPFMC for others</t>
-  </si>
-  <si>
-    <t>age/length based maturity</t>
-  </si>
-  <si>
-    <t>random effects (not coded in yet)</t>
-  </si>
-  <si>
-    <t>all to one area</t>
-  </si>
-  <si>
-    <t>penalized (not operational)</t>
-  </si>
-  <si>
-    <t>terminal year surv biom proportions (not operational)</t>
-  </si>
-  <si>
-    <t>non-expon wt age/length based (not operational)</t>
-  </si>
-  <si>
     <t>current.props1</t>
   </si>
   <si>
@@ -707,7 +662,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -743,12 +698,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -863,7 +812,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -915,7 +864,6 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="40" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1523,7 +1471,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1537,7 +1485,7 @@
         <v>8.5848583971778929</v>
       </c>
       <c r="D2" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="E2" s="1">
         <v>2.15</v>
@@ -1741,7 +1689,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1761,7 +1709,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H2" s="12">
         <v>0.83268153466700001</v>
@@ -1787,7 +1735,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F3" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H3" s="13">
         <v>0.88417999999999997</v>
@@ -1809,7 +1757,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -1831,7 +1779,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F5" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H5" s="12">
         <v>0.83268153466700001</v>
@@ -1857,7 +1805,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F6" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H6" s="13">
         <v>0.88417999999999997</v>
@@ -1879,7 +1827,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -1901,7 +1849,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F8" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H8" s="12">
         <v>0.83268153466700001</v>
@@ -1927,7 +1875,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F9" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H9" s="13">
         <v>0.88417999999999997</v>
@@ -1949,7 +1897,7 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -1971,7 +1919,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H11" s="12">
         <v>0.83268153466700001</v>
@@ -1997,7 +1945,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F12" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H12" s="13">
         <v>0.88417999999999997</v>
@@ -2019,7 +1967,7 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -2041,7 +1989,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F14" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H14" s="12">
         <v>0.83268153466700001</v>
@@ -2067,7 +2015,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F15" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H15" s="13">
         <v>0.88417999999999997</v>
@@ -2089,7 +2037,7 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -2111,7 +2059,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F17" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H17" s="12">
         <v>0.83268153466700001</v>
@@ -2137,7 +2085,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F18" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H18" s="13">
         <v>0.88417999999999997</v>
@@ -2159,7 +2107,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -2181,7 +2129,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F20" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H20" s="20">
         <v>0.85317342242799998</v>
@@ -2207,7 +2155,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F21" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H21" s="20">
         <v>0.88417999999999997</v>
@@ -2229,7 +2177,7 @@
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
       <c r="F22" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
@@ -2251,7 +2199,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F23" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H23" s="22">
         <v>0.85317342242799998</v>
@@ -2277,7 +2225,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F24" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H24" s="23">
         <v>0.88417999999999997</v>
@@ -2299,7 +2247,7 @@
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
       <c r="F25" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
@@ -2321,7 +2269,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F26" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H26" s="25">
         <v>0.85317342242799998</v>
@@ -2347,7 +2295,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F27" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H27" s="26">
         <v>0.88417999999999997</v>
@@ -2369,7 +2317,7 @@
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
       <c r="F28" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H28" s="27"/>
       <c r="I28" s="27"/>
@@ -2391,7 +2339,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F29" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H29" s="27">
         <v>1.1324375825599999</v>
@@ -2417,7 +2365,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F30" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H30" s="26">
         <v>0.88417999999999997</v>
@@ -2439,7 +2387,7 @@
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
       <c r="F31" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
@@ -2461,7 +2409,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F32" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H32" s="25">
         <v>1.4339075566299999</v>
@@ -2487,7 +2435,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F33" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H33" s="26">
         <v>0.88417999999999997</v>
@@ -2509,7 +2457,7 @@
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
       <c r="F34" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H34" s="27"/>
       <c r="I34" s="27"/>
@@ -2531,7 +2479,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F35" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H35" s="25">
         <v>1.4339075566299999</v>
@@ -2557,7 +2505,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F36" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H36" s="26">
         <v>0.88417999999999997</v>
@@ -2579,7 +2527,7 @@
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
       <c r="F37" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
@@ -2619,7 +2567,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F39" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H39" s="12">
         <v>1.4069980317499999</v>
@@ -2645,7 +2593,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F40" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H40" s="12">
         <v>1.74173878351</v>
@@ -2667,7 +2615,7 @@
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -2689,7 +2637,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F42" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H42" s="12">
         <v>1.4069980317499999</v>
@@ -2715,7 +2663,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F43" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H43" s="12">
         <v>1.74173878351</v>
@@ -2737,7 +2685,7 @@
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="F44" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
@@ -2759,7 +2707,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F45" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H45" s="12">
         <v>1.4069980317499999</v>
@@ -2785,7 +2733,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F46" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H46" s="12">
         <v>1.74173878351</v>
@@ -2807,7 +2755,7 @@
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="9"/>
@@ -2829,7 +2777,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F48" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H48" s="12">
         <v>1.4069980317499999</v>
@@ -2855,7 +2803,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F49" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H49" s="12">
         <v>1.74173878351</v>
@@ -2877,7 +2825,7 @@
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
@@ -2899,7 +2847,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F51" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H51" s="12">
         <v>1.4069980317499999</v>
@@ -2925,7 +2873,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F52" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H52" s="12">
         <v>1.74173878351</v>
@@ -2947,7 +2895,7 @@
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
@@ -2969,7 +2917,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F54" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H54" s="12">
         <v>1.4069980317499999</v>
@@ -2995,7 +2943,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F55" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H55" s="12">
         <v>1.74173878351</v>
@@ -3021,7 +2969,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F56" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H56" s="14">
         <v>2.1</v>
@@ -3047,7 +2995,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F57" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H57" s="14">
         <v>0.78649999999999998</v>
@@ -3069,7 +3017,7 @@
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
       <c r="F58" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
@@ -3091,7 +3039,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F59" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H59" s="14">
         <v>2.1</v>
@@ -3117,7 +3065,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F60" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H60" s="14">
         <v>0.78649999999999998</v>
@@ -3139,7 +3087,7 @@
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
       <c r="F61" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
@@ -3161,7 +3109,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F62" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H62" s="14">
         <v>2.1</v>
@@ -3187,7 +3135,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F63" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H63" s="14">
         <v>0.78649999999999998</v>
@@ -3209,7 +3157,7 @@
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
       <c r="F64" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H64" s="15"/>
       <c r="I64" s="15"/>
@@ -3231,7 +3179,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F65" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H65" s="14">
         <v>2.1</v>
@@ -3257,7 +3205,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F66" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H66" s="14">
         <v>0.78649999999999998</v>
@@ -3279,7 +3227,7 @@
       <c r="D67" s="15"/>
       <c r="E67" s="15"/>
       <c r="F67" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="15"/>
@@ -3301,7 +3249,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F68" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H68" s="14">
         <v>2.1</v>
@@ -3327,7 +3275,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F69" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H69" s="14">
         <v>0.78649999999999998</v>
@@ -3349,7 +3297,7 @@
       <c r="D70" s="15"/>
       <c r="E70" s="15"/>
       <c r="F70" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H70" s="15"/>
       <c r="I70" s="15"/>
@@ -3371,7 +3319,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F71" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H71" s="14">
         <v>2.1</v>
@@ -3397,7 +3345,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F72" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H72" s="14">
         <v>0.78649999999999998</v>
@@ -3419,7 +3367,7 @@
       <c r="D73" s="15"/>
       <c r="E73" s="15"/>
       <c r="F73" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H73" s="15"/>
       <c r="I73" s="15"/>
@@ -3597,7 +3545,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3611,7 +3559,7 @@
         <v>5.5123462978056237</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="E2" s="1">
         <v>1.7069903579000001</v>
@@ -26842,10 +26790,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26853,7 +26801,7 @@
     <col min="1" max="1" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -26863,28 +26811,19 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -26894,14 +26833,8 @@
       <c r="C3" t="s">
         <v>129</v>
       </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>127</v>
       </c>
@@ -26911,31 +26844,19 @@
       <c r="C4" t="s">
         <v>128</v>
       </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -26945,241 +26866,181 @@
       <c r="C6" t="s">
         <v>132</v>
       </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-      <c r="J6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B7">
         <v>0.1</v>
       </c>
       <c r="C7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="J7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B8">
         <v>0.13</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I8">
-        <v>7</v>
-      </c>
-      <c r="J8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B9">
         <v>0.11</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
-      <c r="J9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B10">
         <v>0.34</v>
       </c>
       <c r="C10" t="s">
-        <v>154</v>
-      </c>
-      <c r="I10">
-        <v>9</v>
-      </c>
-      <c r="J10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B11">
         <v>0.11</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
-      </c>
-      <c r="I11">
-        <v>10</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B12">
         <v>0.21</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
-      </c>
-      <c r="I12">
-        <v>11</v>
-      </c>
-      <c r="J12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B13">
         <v>9.2315344999999993E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>161</v>
-      </c>
-      <c r="I13">
-        <v>12</v>
-      </c>
-      <c r="J13" s="29" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B14">
         <v>0.13670328400000001</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
-      </c>
-      <c r="I14">
-        <v>13</v>
-      </c>
-      <c r="J14" s="29" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="B15">
         <v>0.13052393000000001</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
-      </c>
-      <c r="I15">
-        <v>14</v>
-      </c>
-      <c r="J15" s="29" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B16">
         <v>0.26827582300000002</v>
       </c>
       <c r="C16" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="B17">
         <v>0.137707199</v>
       </c>
       <c r="C17" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="B18">
         <v>0.23447441899999999</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B19">
         <v>0.1</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="B20">
         <v>0.1</v>
       </c>
       <c r="C20" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B21">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -27818,7 +27679,7 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -27835,7 +27696,7 @@
         <v>3.2118239768019823</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="I2" s="1">
         <v>1.1789042974999999</v>
@@ -27858,7 +27719,7 @@
         <v>4.7114701825907419</v>
       </c>
       <c r="E3" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="I3" s="1">
         <v>1.75</v>
@@ -27877,7 +27738,7 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -27896,7 +27757,7 @@
         <v>7.3890560989306504</v>
       </c>
       <c r="E5" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="I5" s="1">
         <v>0.95670999999999995</v>
@@ -27919,7 +27780,7 @@
         <v>2.2802840077239361</v>
       </c>
       <c r="E6" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
@@ -27938,7 +27799,7 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>

</xml_diff>

<commit_message>
reran sim with dana's changes, added more perf measures code
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -26793,7 +26793,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26817,7 +26817,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -26861,7 +26861,7 @@
         <v>131</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>132</v>

</xml_diff>

<commit_message>
conditioning period seems right, finally. I hope.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -28,6 +28,7 @@
     <sheet name="qFishery" sheetId="15" r:id="rId14"/>
     <sheet name="Movement" sheetId="16" r:id="rId15"/>
     <sheet name="Conditioning_recruitment" sheetId="20" r:id="rId16"/>
+    <sheet name="2018apportionment" sheetId="21" r:id="rId17"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3798" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3826" uniqueCount="170">
   <si>
     <t>Par</t>
   </si>
@@ -461,12 +462,6 @@
     <t>Nstart</t>
   </si>
   <si>
-    <t>Starting numbers (millions) check units</t>
-  </si>
-  <si>
-    <t>Starting biomass (kt) check units (which is 396,000,000 kg)</t>
-  </si>
-  <si>
     <t>Average log-recruitment (either 16.5 or 19.5) - WHAT ARE UNITS?? Million?</t>
   </si>
   <si>
@@ -553,11 +548,53 @@
   <si>
     <t>input value for option 11 - the lucky area that gets 100% of ABC (in order 1:6 BS AI WG CG WY EY/SEO)</t>
   </si>
+  <si>
+    <t>approx LL-trawl split proportion</t>
+  </si>
+  <si>
+    <t>Fixed gear abc</t>
+  </si>
+  <si>
+    <t>trawl abc</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>75-25</t>
+  </si>
+  <si>
+    <t>90-10</t>
+  </si>
+  <si>
+    <t>EY/SEO</t>
+  </si>
+  <si>
+    <t>conf value removed</t>
+  </si>
+  <si>
+    <t>2018 SAFE report apportionment for 2019 (before whales) for sablefish in tons</t>
+  </si>
+  <si>
+    <t>in kt</t>
+  </si>
+  <si>
+    <t>2018 catch for use in apportionment in kt</t>
+  </si>
+  <si>
+    <t>Starting numbers (millions) check units from 2018 MGMT model 1977 N</t>
+  </si>
+  <si>
+    <t>Starting biomass (kt, which is 396,000,000 kg), 2018 mgmt EM tot_biom for 1977</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -812,7 +849,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -864,6 +901,16 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="40" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1471,7 +1518,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,7 +1532,7 @@
         <v>8.5848583971778929</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E2" s="1">
         <v>2.15</v>
@@ -1689,7 +1736,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1709,7 +1756,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H2" s="12">
         <v>0.83268153466700001</v>
@@ -1735,7 +1782,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H3" s="13">
         <v>0.88417999999999997</v>
@@ -1757,7 +1804,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -1779,7 +1826,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H5" s="12">
         <v>0.83268153466700001</v>
@@ -1805,7 +1852,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H6" s="13">
         <v>0.88417999999999997</v>
@@ -1827,7 +1874,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -1849,7 +1896,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H8" s="12">
         <v>0.83268153466700001</v>
@@ -1875,7 +1922,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H9" s="13">
         <v>0.88417999999999997</v>
@@ -1897,7 +1944,7 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -1919,7 +1966,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H11" s="12">
         <v>0.83268153466700001</v>
@@ -1945,7 +1992,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H12" s="13">
         <v>0.88417999999999997</v>
@@ -1967,7 +2014,7 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1989,7 +2036,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H14" s="12">
         <v>0.83268153466700001</v>
@@ -2015,7 +2062,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H15" s="13">
         <v>0.88417999999999997</v>
@@ -2037,7 +2084,7 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -2059,7 +2106,7 @@
         <v>9.8205935562528204</v>
       </c>
       <c r="F17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H17" s="12">
         <v>0.83268153466700001</v>
@@ -2085,7 +2132,7 @@
         <v>1.6718653849036007</v>
       </c>
       <c r="F18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H18" s="13">
         <v>0.88417999999999997</v>
@@ -2107,7 +2154,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -2129,7 +2176,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H20" s="20">
         <v>0.85317342242799998</v>
@@ -2155,7 +2202,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H21" s="20">
         <v>0.88417999999999997</v>
@@ -2177,7 +2224,7 @@
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
       <c r="F22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
@@ -2199,7 +2246,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H23" s="22">
         <v>0.85317342242799998</v>
@@ -2225,7 +2272,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H24" s="23">
         <v>0.88417999999999997</v>
@@ -2247,7 +2294,7 @@
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
       <c r="F25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
@@ -2269,7 +2316,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H26" s="25">
         <v>0.85317342242799998</v>
@@ -2295,7 +2342,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H27" s="26">
         <v>0.88417999999999997</v>
@@ -2317,7 +2364,7 @@
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
       <c r="F28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H28" s="27"/>
       <c r="I28" s="27"/>
@@ -2339,7 +2386,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H29" s="27">
         <v>1.1324375825599999</v>
@@ -2365,7 +2412,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H30" s="26">
         <v>0.88417999999999997</v>
@@ -2387,7 +2434,7 @@
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
       <c r="F31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
@@ -2409,7 +2456,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H32" s="25">
         <v>1.4339075566299999</v>
@@ -2435,7 +2482,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H33" s="26">
         <v>0.88417999999999997</v>
@@ -2457,7 +2504,7 @@
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
       <c r="F34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H34" s="27"/>
       <c r="I34" s="27"/>
@@ -2479,7 +2526,7 @@
         <v>2.2986856730216711</v>
       </c>
       <c r="F35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H35" s="25">
         <v>1.4339075566299999</v>
@@ -2505,7 +2552,7 @@
         <v>3.1478153783457579</v>
       </c>
       <c r="F36" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H36" s="26">
         <v>0.88417999999999997</v>
@@ -2527,7 +2574,7 @@
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
       <c r="F37" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
@@ -2567,7 +2614,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F39" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H39" s="12">
         <v>1.4069980317499999</v>
@@ -2593,7 +2640,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F40" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H40" s="12">
         <v>1.74173878351</v>
@@ -2615,7 +2662,7 @@
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -2637,7 +2684,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F42" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H42" s="12">
         <v>1.4069980317499999</v>
@@ -2663,7 +2710,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F43" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H43" s="12">
         <v>1.74173878351</v>
@@ -2685,7 +2732,7 @@
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="F44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
@@ -2707,7 +2754,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F45" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H45" s="12">
         <v>1.4069980317499999</v>
@@ -2733,7 +2780,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F46" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H46" s="12">
         <v>1.74173878351</v>
@@ -2755,7 +2802,7 @@
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="9"/>
@@ -2777,7 +2824,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F48" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H48" s="12">
         <v>1.4069980317499999</v>
@@ -2803,7 +2850,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F49" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H49" s="12">
         <v>1.74173878351</v>
@@ -2825,7 +2872,7 @@
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
@@ -2847,7 +2894,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H51" s="12">
         <v>1.4069980317499999</v>
@@ -2873,7 +2920,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F52" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H52" s="12">
         <v>1.74173878351</v>
@@ -2895,7 +2942,7 @@
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
@@ -2917,7 +2964,7 @@
         <v>3.8168785874624138</v>
       </c>
       <c r="F54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H54" s="12">
         <v>1.4069980317499999</v>
@@ -2943,7 +2990,7 @@
         <v>5.7072584870432808</v>
       </c>
       <c r="F55" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H55" s="12">
         <v>1.74173878351</v>
@@ -2969,7 +3016,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F56" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H56" s="14">
         <v>2.1</v>
@@ -2995,7 +3042,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F57" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H57" s="14">
         <v>0.78649999999999998</v>
@@ -3017,7 +3064,7 @@
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
       <c r="F58" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
@@ -3039,7 +3086,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F59" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H59" s="14">
         <v>2.1</v>
@@ -3065,7 +3112,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F60" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H60" s="14">
         <v>0.78649999999999998</v>
@@ -3087,7 +3134,7 @@
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
       <c r="F61" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
@@ -3109,7 +3156,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F62" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H62" s="14">
         <v>2.1</v>
@@ -3135,7 +3182,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F63" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H63" s="14">
         <v>0.78649999999999998</v>
@@ -3157,7 +3204,7 @@
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
       <c r="F64" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H64" s="15"/>
       <c r="I64" s="15"/>
@@ -3179,7 +3226,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F65" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H65" s="14">
         <v>2.1</v>
@@ -3205,7 +3252,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F66" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H66" s="14">
         <v>0.78649999999999998</v>
@@ -3227,7 +3274,7 @@
       <c r="D67" s="15"/>
       <c r="E67" s="15"/>
       <c r="F67" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="15"/>
@@ -3249,7 +3296,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F68" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H68" s="14">
         <v>2.1</v>
@@ -3275,7 +3322,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F69" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H69" s="14">
         <v>0.78649999999999998</v>
@@ -3297,7 +3344,7 @@
       <c r="D70" s="15"/>
       <c r="E70" s="15"/>
       <c r="F70" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H70" s="15"/>
       <c r="I70" s="15"/>
@@ -3319,7 +3366,7 @@
         <v>8.1661699125676517</v>
       </c>
       <c r="F71" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H71" s="14">
         <v>2.1</v>
@@ -3345,7 +3392,7 @@
         <v>2.1956980188358153</v>
       </c>
       <c r="F72" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H72" s="14">
         <v>0.78649999999999998</v>
@@ -3367,7 +3414,7 @@
       <c r="D73" s="15"/>
       <c r="E73" s="15"/>
       <c r="F73" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H73" s="15"/>
       <c r="I73" s="15"/>
@@ -3545,7 +3592,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3559,7 +3606,7 @@
         <v>5.5123462978056237</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E2" s="1">
         <v>1.7069903579000001</v>
@@ -26788,6 +26835,309 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3">
+        <v>1501</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3">
+        <f>B3*0.75</f>
+        <v>1125.75</v>
+      </c>
+      <c r="E3">
+        <f>B3-D3</f>
+        <v>375.25</v>
+      </c>
+      <c r="G3">
+        <f>SUM(D3:E3)</f>
+        <v>1501</v>
+      </c>
+      <c r="J3">
+        <f>D3/1000</f>
+        <v>1.12575</v>
+      </c>
+      <c r="K3">
+        <f>E3/1000</f>
+        <v>0.37524999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4">
+        <v>2030</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4">
+        <f>B4*0.75</f>
+        <v>1522.5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E8" si="0">B4-D4</f>
+        <v>507.5</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G8" si="1">SUM(D4:E4)</f>
+        <v>2030</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:K8" si="2">D4/1000</f>
+        <v>1.5225</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>0.50749999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5">
+        <v>1659</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5">
+        <f>B5*0.9</f>
+        <v>1493.1000000000001</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>165.89999999999986</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>1659</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>1.4931000000000001</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>0.16589999999999985</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6">
+        <v>5246</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6">
+        <f>B6*0.9</f>
+        <v>4721.4000000000005</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>524.59999999999945</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>5246</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>4.7214000000000009</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>0.5245999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7">
+        <v>1765</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7">
+        <f>B7*0.9</f>
+        <v>1588.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>176.5</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>1765</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>1.5885</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>0.17649999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8">
+        <v>3179</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8">
+        <f>B8*0.9</f>
+        <v>2861.1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>317.90000000000009</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>3179</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>2.8611</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>0.31790000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="31">
+        <v>0.52981632243900001</v>
+      </c>
+      <c r="E12" s="32">
+        <v>1.0684274691339002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="31">
+        <v>0.48119124231240001</v>
+      </c>
+      <c r="E13" s="31">
+        <v>0.17887271999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="31">
+        <v>1.1777329293090988</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0.22376370702149997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="31">
+        <v>3.6386658550291102</v>
+      </c>
+      <c r="E15" s="31">
+        <v>2.1308782359282001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="31">
+        <v>1.6230855103830002</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="31">
+        <v>3.0081467753727003</v>
+      </c>
+      <c r="E17" s="31">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
@@ -26817,7 +27167,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -26827,11 +27177,11 @@
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2">
-        <v>396</v>
+      <c r="B3" s="34">
+        <v>295.01400000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -26839,10 +27189,10 @@
         <v>127</v>
       </c>
       <c r="B4" s="2">
-        <v>111.157</v>
+        <v>93.41</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -26850,7 +27200,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -26858,189 +27208,189 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7">
         <v>0.1</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B8">
         <v>0.13</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9">
         <v>0.11</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B10">
         <v>0.34</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B11">
         <v>0.11</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B12">
         <v>0.21</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B13">
         <v>9.2315344999999993E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B14">
         <v>0.13670328400000001</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B15">
         <v>0.13052393000000001</v>
       </c>
       <c r="C15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B16">
         <v>0.26827582300000002</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B17">
         <v>0.137707199</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B18">
         <v>0.23447441899999999</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B19">
         <v>0.1</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B20">
         <v>0.1</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B21">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -27559,7 +27909,7 @@
         <v>16.5</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -27679,7 +28029,7 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -27696,7 +28046,7 @@
         <v>3.2118239768019823</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I2" s="1">
         <v>1.1789042974999999</v>
@@ -27719,7 +28069,7 @@
         <v>4.7114701825907419</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I3" s="1">
         <v>1.75</v>
@@ -27738,7 +28088,7 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -27757,7 +28107,7 @@
         <v>7.3890560989306504</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I5" s="1">
         <v>0.95670999999999995</v>
@@ -27780,7 +28130,7 @@
         <v>2.2802840077239361</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
@@ -27799,7 +28149,7 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>

</xml_diff>

<commit_message>
fixed the report code in tpl
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -27143,7 +27143,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -27167,7 +27167,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -27200,7 +27200,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
added more plots and text to rmd file.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -27143,7 +27143,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -27211,7 +27211,7 @@
         <v>129</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
more performance metrics and figures for the rmd code
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -27167,7 +27167,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -27200,7 +27200,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -27211,7 +27211,7 @@
         <v>129</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
tweaked the output (save.rds) for natage since it was too big for my computer to do anything with it...
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="1"/>
+    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -1708,7 +1708,7 @@
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E3"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1750,7 +1750,7 @@
         <v>48</v>
       </c>
       <c r="D2" s="12">
-        <v>2.299476606544725</v>
+        <v>2.2994766065447201</v>
       </c>
       <c r="E2" s="12">
         <v>9.8205935562528204</v>
@@ -2380,10 +2380,10 @@
         <v>48</v>
       </c>
       <c r="D29" s="22">
-        <v>2.3470833330266236</v>
+        <v>3.103211622797875</v>
       </c>
       <c r="E29" s="22">
-        <v>2.2986856730216711</v>
+        <v>3.2422654255153662</v>
       </c>
       <c r="F29" t="s">
         <v>152</v>
@@ -2450,10 +2450,10 @@
         <v>48</v>
       </c>
       <c r="D32" s="22">
-        <v>2.3470833330266236</v>
+        <v>4.1950596395258719</v>
       </c>
       <c r="E32" s="22">
-        <v>2.2986856730216711</v>
+        <v>3.6583649259835629</v>
       </c>
       <c r="F32" t="s">
         <v>152</v>
@@ -2520,10 +2520,10 @@
         <v>48</v>
       </c>
       <c r="D35" s="22">
-        <v>2.3470833330266236</v>
+        <v>4.1950596395258719</v>
       </c>
       <c r="E35" s="22">
-        <v>2.2986856730216711</v>
+        <v>3.6583649259835629</v>
       </c>
       <c r="F35" t="s">
         <v>152</v>
@@ -27142,8 +27142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -27167,7 +27167,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -27200,7 +27200,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -27211,7 +27211,7 @@
         <v>129</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>130</v>
@@ -28003,8 +28003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -28040,19 +28040,19 @@
         <v>48</v>
       </c>
       <c r="C2" s="1">
-        <v>3.250810329768528</v>
+        <v>3.2657844689173556</v>
       </c>
       <c r="D2" s="1">
-        <v>3.2118239768019823</v>
+        <v>3.1892953532553738</v>
       </c>
       <c r="E2" t="s">
         <v>152</v>
       </c>
       <c r="I2" s="1">
-        <v>1.1789042974999999</v>
+        <v>1.1835</v>
       </c>
       <c r="J2" s="1">
-        <v>1.16683899284</v>
+        <v>1.1597999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -28101,19 +28101,19 @@
         <v>48</v>
       </c>
       <c r="C5" s="1">
-        <v>2.6031181111692159</v>
+        <v>2.7625653978402638</v>
       </c>
       <c r="D5" s="1">
-        <v>7.3890560989306504</v>
+        <v>3.5993351873576613</v>
       </c>
       <c r="E5" t="s">
         <v>152</v>
       </c>
       <c r="I5" s="1">
-        <v>0.95670999999999995</v>
+        <v>1.01615973999</v>
       </c>
       <c r="J5" s="1">
-        <v>2</v>
+        <v>1.2807491582299999</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -28124,19 +28124,19 @@
         <v>49</v>
       </c>
       <c r="C6" s="1">
-        <v>2.7182818284590451</v>
+        <v>1.7862024155430378</v>
       </c>
       <c r="D6" s="1">
-        <v>2.2802840077239361</v>
+        <v>1.7862024155430378</v>
       </c>
       <c r="E6" t="s">
         <v>152</v>
       </c>
       <c r="I6" s="1">
-        <v>1</v>
+        <v>0.58009181060299997</v>
       </c>
       <c r="J6" s="1">
-        <v>0.82430000000000003</v>
+        <v>0.58009181060299997</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
started adding code to sort out non-converged or crashed runs
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input.xlsx
+++ b/data/Sablefish_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="43680" yWindow="2760" windowWidth="38400" windowHeight="22620" tabRatio="767" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27143,7 +27143,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -27167,7 +27167,7 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -27200,7 +27200,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -27884,7 +27884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -27917,7 +27917,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
@@ -28003,8 +28003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:M1048576"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>